<commit_message>
Add tests for return_accumulate
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\SAS_Perf_Anly\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qiyuan\Documents\GitHub\SASPerformanceAnalytics\Performance Analytics Library\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="8000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Test</t>
   </si>
@@ -294,6 +294,60 @@
   </si>
   <si>
     <t>Msquared_test1</t>
+  </si>
+  <si>
+    <t>Return_accumulate1</t>
+  </si>
+  <si>
+    <t>Test simple return aggregated monthly</t>
+  </si>
+  <si>
+    <t>return_accumulate_test1</t>
+  </si>
+  <si>
+    <t>Return_accumulate2</t>
+  </si>
+  <si>
+    <t>Test compound return aggregated monthly</t>
+  </si>
+  <si>
+    <t>return_accumulate_test2</t>
+  </si>
+  <si>
+    <t>Return_accumulate3</t>
+  </si>
+  <si>
+    <t>Test simple return aggregated quarterly</t>
+  </si>
+  <si>
+    <t>return_accumulate_test3</t>
+  </si>
+  <si>
+    <t>Return_accumulate4</t>
+  </si>
+  <si>
+    <t>Test compound return aggregated quarterly</t>
+  </si>
+  <si>
+    <t>return_accumulate_test4</t>
+  </si>
+  <si>
+    <t>Return_accumulate5</t>
+  </si>
+  <si>
+    <t>return_accumulate_test5</t>
+  </si>
+  <si>
+    <t>Return_accumulate6</t>
+  </si>
+  <si>
+    <t>return_accumulate_test6</t>
+  </si>
+  <si>
+    <t>Test simple return aggregated yearly</t>
+  </si>
+  <si>
+    <t>Test compound return aggregated yearly</t>
   </si>
 </sst>
 </file>
@@ -333,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -349,7 +403,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -611,20 +665,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -646,7 +700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -657,7 +711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -668,7 +722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -679,7 +733,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -690,7 +744,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -701,7 +755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -712,7 +766,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -723,7 +777,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -734,7 +788,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -745,7 +799,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -756,7 +810,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -767,7 +821,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -778,7 +832,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -789,7 +843,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -800,7 +854,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -811,7 +865,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -822,7 +876,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -833,7 +887,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -844,7 +898,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -855,7 +909,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -866,7 +920,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -877,7 +931,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -888,7 +942,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -899,7 +953,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -910,7 +964,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -921,7 +975,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -932,7 +986,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -943,7 +997,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -952,6 +1006,72 @@
       </c>
       <c r="C30" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test1 for scalar_annualized
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Test</t>
   </si>
@@ -348,6 +348,15 @@
   </si>
   <si>
     <t>Test compound return aggregated yearly</t>
+  </si>
+  <si>
+    <t>Scalar_annualized1</t>
+  </si>
+  <si>
+    <t>Test scalar annulized for value</t>
+  </si>
+  <si>
+    <t>scalar_annualized_test1</t>
   </si>
 </sst>
 </file>
@@ -665,15 +674,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1074,6 +1083,17 @@
         <v>105</v>
       </c>
     </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add tests for scalar_annualized
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>Test</t>
   </si>
@@ -353,10 +353,28 @@
     <t>Scalar_annualized1</t>
   </si>
   <si>
-    <t>Test scalar annulized for value</t>
-  </si>
-  <si>
     <t>scalar_annualized_test1</t>
+  </si>
+  <si>
+    <t>Scalar_annualized2</t>
+  </si>
+  <si>
+    <t>scalar_annualized_test2</t>
+  </si>
+  <si>
+    <t>Test scalar annulized for discrete value</t>
+  </si>
+  <si>
+    <t>Scalar_annualized3</t>
+  </si>
+  <si>
+    <t>Test scalar annulized for log value</t>
+  </si>
+  <si>
+    <t>scalar_annualized_test3</t>
+  </si>
+  <si>
+    <t>Test scalar annulized for std</t>
   </si>
 </sst>
 </file>
@@ -674,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1088,10 +1106,32 @@
         <v>108</v>
       </c>
       <c r="B37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" t="s">
         <v>109</v>
       </c>
-      <c r="C37" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>110</v>
+      </c>
+      <c r="B38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test for Treynor_Ratio macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qiyuan\Documents\GitHub\SASPerformanceAnalytics\Performance Analytics Library\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="8000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19716" windowHeight="8004"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Test</t>
   </si>
@@ -375,6 +370,15 @@
   </si>
   <si>
     <t>Test scalar annulized for std</t>
+  </si>
+  <si>
+    <t>Treynor Ratio1</t>
+  </si>
+  <si>
+    <t>Test Treynor Ratio</t>
+  </si>
+  <si>
+    <t>Treynor_Ratio_test1</t>
   </si>
 </sst>
 </file>
@@ -414,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -472,7 +476,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -507,7 +511,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -684,7 +688,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -692,17 +696,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1134,6 +1138,17 @@
         <v>115</v>
       </c>
     </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add test to Bull_Bear_beta macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>Test</t>
   </si>
@@ -388,6 +388,15 @@
   </si>
   <si>
     <t>Systematic Risk1</t>
+  </si>
+  <si>
+    <t>Bull/Bear beta1</t>
+  </si>
+  <si>
+    <t>Test bull/bear beta</t>
+  </si>
+  <si>
+    <t>Bull_Bear_beta_test1</t>
   </si>
 </sst>
 </file>
@@ -697,7 +706,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -705,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,7 +947,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -949,7 +958,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -960,7 +969,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -971,7 +980,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -982,7 +991,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -993,7 +1002,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1004,7 +1013,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -1015,7 +1024,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -1026,7 +1035,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -1037,7 +1046,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -1048,7 +1057,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -1059,7 +1068,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -1070,7 +1079,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>96</v>
       </c>
@@ -1081,7 +1090,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>99</v>
       </c>
@@ -1092,7 +1101,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -1103,7 +1112,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>110</v>
       </c>
@@ -1136,7 +1145,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>113</v>
       </c>
@@ -1167,6 +1176,17 @@
       </c>
       <c r="C41" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test to table_CAPM
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>Test</t>
   </si>
@@ -397,6 +397,15 @@
   </si>
   <si>
     <t>Bull_Bear_beta_test1</t>
+  </si>
+  <si>
+    <t>table_CAPM1</t>
+  </si>
+  <si>
+    <t>Test CAPM table</t>
+  </si>
+  <si>
+    <t>table_CAPM_test1</t>
   </si>
 </sst>
 </file>
@@ -706,7 +715,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -714,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,6 +1198,17 @@
         <v>125</v>
       </c>
     </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Complete tests for SharpeRatio_annualized macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="154">
   <si>
     <t>Test</t>
   </si>
@@ -111,301 +111,376 @@
     <t>Standard_Deviation_test2</t>
   </si>
   <si>
-    <t>Test Sharpe Ratio Annualized</t>
-  </si>
-  <si>
-    <t>Sharpe Ratio1</t>
-  </si>
-  <si>
     <t>SharpeRatio_annualized_test1</t>
   </si>
   <si>
+    <t>SharpeRatio_annualized_test2</t>
+  </si>
+  <si>
+    <t>Annualized Returns Table</t>
+  </si>
+  <si>
+    <t>Test Annualized table</t>
+  </si>
+  <si>
+    <t>table_Annualized_Returns_test1</t>
+  </si>
+  <si>
+    <t>CAPM_alpha_beta_test1</t>
+  </si>
+  <si>
+    <t>CAPM_alpha_beta</t>
+  </si>
+  <si>
+    <t>Test alpha and beta values</t>
+  </si>
+  <si>
+    <t>CAPM_epsilon</t>
+  </si>
+  <si>
+    <t>Test error term</t>
+  </si>
+  <si>
+    <t>CAPM_epsilon_test1</t>
+  </si>
+  <si>
+    <t>Correlation Table</t>
+  </si>
+  <si>
+    <t>Test correlation table</t>
+  </si>
+  <si>
+    <t>table_correlation_test1</t>
+  </si>
+  <si>
+    <t>AutoCorrelation Table</t>
+  </si>
+  <si>
+    <t>Test autocorrelation table</t>
+  </si>
+  <si>
+    <t>table_autocorrelation_test1</t>
+  </si>
+  <si>
+    <t>Table_Stats</t>
+  </si>
+  <si>
+    <t>Test stats table</t>
+  </si>
+  <si>
+    <t>table_stats_test1</t>
+  </si>
+  <si>
+    <t>Table_variability</t>
+  </si>
+  <si>
+    <t>Test variability table</t>
+  </si>
+  <si>
+    <t>table_variability_test1</t>
+  </si>
+  <si>
+    <t>Table_distributions</t>
+  </si>
+  <si>
+    <t>Test distributions table</t>
+  </si>
+  <si>
+    <t>table_distributions_test1</t>
+  </si>
+  <si>
+    <t>Table_HigherMoments</t>
+  </si>
+  <si>
+    <t>Test Higher Moments table</t>
+  </si>
+  <si>
+    <t>table_HigherMoments_test1</t>
+  </si>
+  <si>
+    <t>Table_InformationRatio</t>
+  </si>
+  <si>
+    <t>Test Information Ratio Table</t>
+  </si>
+  <si>
+    <t>table_InformationRatio_test1</t>
+  </si>
+  <si>
+    <t>Table_SpecificRisk</t>
+  </si>
+  <si>
+    <t>Test Specific Risk</t>
+  </si>
+  <si>
+    <t>table_SpecificRisk_test1</t>
+  </si>
+  <si>
+    <t>Table_CalendarReturns</t>
+  </si>
+  <si>
+    <t>Test Calendar Returns</t>
+  </si>
+  <si>
+    <t>table_CalendarReturns_test1</t>
+  </si>
+  <si>
+    <t>Adjusted_SharpeRatio</t>
+  </si>
+  <si>
+    <t>Test Adjusted Sharpe</t>
+  </si>
+  <si>
+    <t>Adjusted_SharpeRatio_test1</t>
+  </si>
+  <si>
+    <t>ActivePremium</t>
+  </si>
+  <si>
+    <t>Test Active premium</t>
+  </si>
+  <si>
+    <t>ActivePremium_test1</t>
+  </si>
+  <si>
+    <t>fama_beta</t>
+  </si>
+  <si>
+    <t>Test Fama Beta</t>
+  </si>
+  <si>
+    <t>fama_beta_test1</t>
+  </si>
+  <si>
+    <t>appraisal ratio</t>
+  </si>
+  <si>
+    <t>Test appraisal ratio</t>
+  </si>
+  <si>
+    <t>appraisal_ratio_test1</t>
+  </si>
+  <si>
+    <t>CAPM_JensenAlpha</t>
+  </si>
+  <si>
+    <t>Test Jensen Alpha</t>
+  </si>
+  <si>
+    <t>CAPM_JensenAlpha_test1</t>
+  </si>
+  <si>
+    <t>Msquared</t>
+  </si>
+  <si>
+    <t>Test Msquared</t>
+  </si>
+  <si>
+    <t>Msquared_test1</t>
+  </si>
+  <si>
+    <t>Return_accumulate1</t>
+  </si>
+  <si>
+    <t>Test simple return aggregated monthly</t>
+  </si>
+  <si>
+    <t>return_accumulate_test1</t>
+  </si>
+  <si>
+    <t>Return_accumulate2</t>
+  </si>
+  <si>
+    <t>Test compound return aggregated monthly</t>
+  </si>
+  <si>
+    <t>return_accumulate_test2</t>
+  </si>
+  <si>
+    <t>Return_accumulate3</t>
+  </si>
+  <si>
+    <t>Test simple return aggregated quarterly</t>
+  </si>
+  <si>
+    <t>return_accumulate_test3</t>
+  </si>
+  <si>
+    <t>Return_accumulate4</t>
+  </si>
+  <si>
+    <t>Test compound return aggregated quarterly</t>
+  </si>
+  <si>
+    <t>return_accumulate_test4</t>
+  </si>
+  <si>
+    <t>Return_accumulate5</t>
+  </si>
+  <si>
+    <t>return_accumulate_test5</t>
+  </si>
+  <si>
+    <t>Return_accumulate6</t>
+  </si>
+  <si>
+    <t>return_accumulate_test6</t>
+  </si>
+  <si>
+    <t>Test simple return aggregated yearly</t>
+  </si>
+  <si>
+    <t>Test compound return aggregated yearly</t>
+  </si>
+  <si>
+    <t>Scalar_annualized1</t>
+  </si>
+  <si>
+    <t>scalar_annualized_test1</t>
+  </si>
+  <si>
+    <t>Scalar_annualized2</t>
+  </si>
+  <si>
+    <t>scalar_annualized_test2</t>
+  </si>
+  <si>
+    <t>Test scalar annulized for discrete value</t>
+  </si>
+  <si>
+    <t>Scalar_annualized3</t>
+  </si>
+  <si>
+    <t>Test scalar annulized for log value</t>
+  </si>
+  <si>
+    <t>scalar_annualized_test3</t>
+  </si>
+  <si>
+    <t>Test scalar annulized for std</t>
+  </si>
+  <si>
+    <t>Treynor Ratio1</t>
+  </si>
+  <si>
+    <t>Test Treynor Ratio</t>
+  </si>
+  <si>
+    <t>Treynor_Ratio_test1</t>
+  </si>
+  <si>
+    <t>Systematic_Risk_test1</t>
+  </si>
+  <si>
+    <t>Test Systematic Risk</t>
+  </si>
+  <si>
+    <t>Systematic Risk1</t>
+  </si>
+  <si>
+    <t>Bull/Bear beta1</t>
+  </si>
+  <si>
+    <t>Test bull/bear beta</t>
+  </si>
+  <si>
+    <t>Bull_Bear_beta_test1</t>
+  </si>
+  <si>
+    <t>table_CAPM1</t>
+  </si>
+  <si>
+    <t>Test CAPM table</t>
+  </si>
+  <si>
+    <t>table_CAPM_test1</t>
+  </si>
+  <si>
+    <t>Active premium2</t>
+  </si>
+  <si>
+    <t>Test ActivePremium</t>
+  </si>
+  <si>
+    <t>ActivePremium_test2</t>
+  </si>
+  <si>
+    <t>CAPM_alpha_beta2</t>
+  </si>
+  <si>
+    <t>CAPM_alpha_beta_test2</t>
+  </si>
+  <si>
     <t>Sharpe Ratio2</t>
   </si>
   <si>
-    <t>Test Arithmetic Sharpe Ratio</t>
-  </si>
-  <si>
-    <t>SharpeRatio_annualized_test2</t>
-  </si>
-  <si>
-    <t>Annualized Returns Table</t>
-  </si>
-  <si>
-    <t>Test Annualized table</t>
-  </si>
-  <si>
-    <t>table_Annualized_Returns_test1</t>
-  </si>
-  <si>
-    <t>CAPM_alpha_beta_test1</t>
-  </si>
-  <si>
-    <t>CAPM_alpha_beta</t>
-  </si>
-  <si>
-    <t>Test alpha and beta values</t>
-  </si>
-  <si>
-    <t>CAPM_epsilon</t>
-  </si>
-  <si>
-    <t>Test error term</t>
-  </si>
-  <si>
-    <t>CAPM_epsilon_test1</t>
-  </si>
-  <si>
-    <t>Correlation Table</t>
-  </si>
-  <si>
-    <t>Test correlation table</t>
-  </si>
-  <si>
-    <t>table_correlation_test1</t>
-  </si>
-  <si>
-    <t>AutoCorrelation Table</t>
-  </si>
-  <si>
-    <t>Test autocorrelation table</t>
-  </si>
-  <si>
-    <t>table_autocorrelation_test1</t>
-  </si>
-  <si>
-    <t>Table_Stats</t>
-  </si>
-  <si>
-    <t>Test stats table</t>
-  </si>
-  <si>
-    <t>table_stats_test1</t>
-  </si>
-  <si>
-    <t>Table_variability</t>
-  </si>
-  <si>
-    <t>Test variability table</t>
-  </si>
-  <si>
-    <t>table_variability_test1</t>
-  </si>
-  <si>
-    <t>Table_distributions</t>
-  </si>
-  <si>
-    <t>Test distributions table</t>
-  </si>
-  <si>
-    <t>table_distributions_test1</t>
-  </si>
-  <si>
-    <t>Table_HigherMoments</t>
-  </si>
-  <si>
-    <t>Test Higher Moments table</t>
-  </si>
-  <si>
-    <t>table_HigherMoments_test1</t>
-  </si>
-  <si>
-    <t>Table_InformationRatio</t>
-  </si>
-  <si>
-    <t>Test Information Ratio Table</t>
-  </si>
-  <si>
-    <t>table_InformationRatio_test1</t>
-  </si>
-  <si>
-    <t>Table_SpecificRisk</t>
-  </si>
-  <si>
-    <t>Test Specific Risk</t>
-  </si>
-  <si>
-    <t>table_SpecificRisk_test1</t>
-  </si>
-  <si>
-    <t>Table_CalendarReturns</t>
-  </si>
-  <si>
-    <t>Test Calendar Returns</t>
-  </si>
-  <si>
-    <t>table_CalendarReturns_test1</t>
-  </si>
-  <si>
-    <t>Adjusted_SharpeRatio</t>
-  </si>
-  <si>
-    <t>Test Adjusted Sharpe</t>
-  </si>
-  <si>
-    <t>Adjusted_SharpeRatio_test1</t>
-  </si>
-  <si>
-    <t>ActivePremium</t>
-  </si>
-  <si>
-    <t>Test Active premium</t>
-  </si>
-  <si>
-    <t>ActivePremium_test1</t>
-  </si>
-  <si>
-    <t>fama_beta</t>
-  </si>
-  <si>
-    <t>Test Fama Beta</t>
-  </si>
-  <si>
-    <t>fama_beta_test1</t>
-  </si>
-  <si>
-    <t>appraisal ratio</t>
-  </si>
-  <si>
-    <t>Test appraisal ratio</t>
-  </si>
-  <si>
-    <t>appraisal_ratio_test1</t>
-  </si>
-  <si>
-    <t>CAPM_JensenAlpha</t>
-  </si>
-  <si>
-    <t>Test Jensen Alpha</t>
-  </si>
-  <si>
-    <t>CAPM_JensenAlpha_test1</t>
-  </si>
-  <si>
-    <t>Msquared</t>
-  </si>
-  <si>
-    <t>Test Msquared</t>
-  </si>
-  <si>
-    <t>Msquared_test1</t>
-  </si>
-  <si>
-    <t>Return_accumulate1</t>
-  </si>
-  <si>
-    <t>Test simple return aggregated monthly</t>
-  </si>
-  <si>
-    <t>return_accumulate_test1</t>
-  </si>
-  <si>
-    <t>Return_accumulate2</t>
-  </si>
-  <si>
-    <t>Test compound return aggregated monthly</t>
-  </si>
-  <si>
-    <t>return_accumulate_test2</t>
-  </si>
-  <si>
-    <t>Return_accumulate3</t>
-  </si>
-  <si>
-    <t>Test simple return aggregated quarterly</t>
-  </si>
-  <si>
-    <t>return_accumulate_test3</t>
-  </si>
-  <si>
-    <t>Return_accumulate4</t>
-  </si>
-  <si>
-    <t>Test compound return aggregated quarterly</t>
-  </si>
-  <si>
-    <t>return_accumulate_test4</t>
-  </si>
-  <si>
-    <t>Return_accumulate5</t>
-  </si>
-  <si>
-    <t>return_accumulate_test5</t>
-  </si>
-  <si>
-    <t>Return_accumulate6</t>
-  </si>
-  <si>
-    <t>return_accumulate_test6</t>
-  </si>
-  <si>
-    <t>Test simple return aggregated yearly</t>
-  </si>
-  <si>
-    <t>Test compound return aggregated yearly</t>
-  </si>
-  <si>
-    <t>Scalar_annualized1</t>
-  </si>
-  <si>
-    <t>scalar_annualized_test1</t>
-  </si>
-  <si>
-    <t>Scalar_annualized2</t>
-  </si>
-  <si>
-    <t>scalar_annualized_test2</t>
-  </si>
-  <si>
-    <t>Test scalar annulized for discrete value</t>
-  </si>
-  <si>
-    <t>Scalar_annualized3</t>
-  </si>
-  <si>
-    <t>Test scalar annulized for log value</t>
-  </si>
-  <si>
-    <t>scalar_annualized_test3</t>
-  </si>
-  <si>
-    <t>Test scalar annulized for std</t>
-  </si>
-  <si>
-    <t>Treynor Ratio1</t>
-  </si>
-  <si>
-    <t>Test Treynor Ratio</t>
-  </si>
-  <si>
-    <t>Treynor_Ratio_test1</t>
-  </si>
-  <si>
-    <t>Systematic_Risk_test1</t>
-  </si>
-  <si>
-    <t>Test Systematic Risk</t>
-  </si>
-  <si>
-    <t>Systematic Risk1</t>
-  </si>
-  <si>
-    <t>Bull/Bear beta1</t>
-  </si>
-  <si>
-    <t>Test bull/bear beta</t>
-  </si>
-  <si>
-    <t>Bull_Bear_beta_test1</t>
-  </si>
-  <si>
-    <t>table_CAPM1</t>
-  </si>
-  <si>
-    <t>Test CAPM table</t>
-  </si>
-  <si>
-    <t>table_CAPM_test1</t>
+    <t>Test Sharpe_Ratio</t>
+  </si>
+  <si>
+    <t>Sharpe_Ratio_test2</t>
+  </si>
+  <si>
+    <t>Annualized StdDev</t>
+  </si>
+  <si>
+    <t>Test StdDev_annualized</t>
+  </si>
+  <si>
+    <t>StdDev_annualized_test1</t>
+  </si>
+  <si>
+    <t>Table_distributions2</t>
+  </si>
+  <si>
+    <t>table_distributions_test2</t>
+  </si>
+  <si>
+    <t>Active premium3</t>
+  </si>
+  <si>
+    <t>ActivePremium_test3</t>
+  </si>
+  <si>
+    <t>Active premium4</t>
+  </si>
+  <si>
+    <t>ActivePremium_test4</t>
+  </si>
+  <si>
+    <t>Sharpe Ratio</t>
+  </si>
+  <si>
+    <t>Sharpe_Ratio_test</t>
+  </si>
+  <si>
+    <t>Sharpe Ratio Annualized1</t>
+  </si>
+  <si>
+    <t>Sharpe Ratio Annualized2</t>
+  </si>
+  <si>
+    <t>Sharpe Ratio Annualized3</t>
+  </si>
+  <si>
+    <t>SharpeRatio_annualized_test3</t>
+  </si>
+  <si>
+    <t>Sharpe Ratio Annualized4</t>
+  </si>
+  <si>
+    <t>SharpeRatio_annualized_test4</t>
+  </si>
+  <si>
+    <t>Test Sharpe Ratio with method=discrete, scale=252</t>
+  </si>
+  <si>
+    <t>Test Sharpe Ratio with method=log, scale=4</t>
+  </si>
+  <si>
+    <t>Test Sharpe Ratio with method=log, scale=12</t>
+  </si>
+  <si>
+    <t>Test Sharpe Ratio with method=discrete, scale=1</t>
   </si>
 </sst>
 </file>
@@ -715,7 +790,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -723,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,265 +921,265 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
         <v>101</v>
@@ -1112,68 +1187,68 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" t="s">
         <v>107</v>
-      </c>
-      <c r="C36" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
         <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
         <v>114</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" t="s">
         <v>116</v>
-      </c>
-      <c r="C39" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B40" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1181,35 +1256,146 @@
         <v>122</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C42" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" t="s">
         <v>126</v>
       </c>
-      <c r="B43" t="s">
-        <v>127</v>
-      </c>
       <c r="C43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" t="s">
+        <v>152</v>
+      </c>
+      <c r="C49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>128</v>
+      </c>
+      <c r="B51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complete tests for CAPM_alpha_beta macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -126,9 +126,6 @@
     <t>table_Annualized_Returns_test1</t>
   </si>
   <si>
-    <t>CAPM_alpha_beta_test1</t>
-  </si>
-  <si>
     <t>CAPM_alpha_beta</t>
   </si>
   <si>
@@ -378,15 +375,9 @@
     <t>Systematic Risk1</t>
   </si>
   <si>
-    <t>Bull/Bear beta1</t>
-  </si>
-  <si>
     <t>Test bull/bear beta</t>
   </si>
   <si>
-    <t>Bull_Bear_beta_test1</t>
-  </si>
-  <si>
     <t>table_CAPM1</t>
   </si>
   <si>
@@ -481,6 +472,15 @@
   </si>
   <si>
     <t>Test Sharpe Ratio with method=discrete, scale=1</t>
+  </si>
+  <si>
+    <t>Bull/Bear beta</t>
+  </si>
+  <si>
+    <t>Bull_Bear_beta_test</t>
+  </si>
+  <si>
+    <t>CAPM_alpha_beta_test</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,384 +934,384 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>57</v>
-      </c>
-      <c r="C19" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
         <v>59</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>60</v>
-      </c>
-      <c r="C20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
         <v>62</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>63</v>
-      </c>
-      <c r="C21" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
         <v>65</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>66</v>
-      </c>
-      <c r="C22" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
         <v>68</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>69</v>
-      </c>
-      <c r="C23" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
         <v>71</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>72</v>
-      </c>
-      <c r="C24" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
         <v>74</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>75</v>
-      </c>
-      <c r="C25" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
         <v>77</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>78</v>
-      </c>
-      <c r="C26" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
         <v>80</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>81</v>
-      </c>
-      <c r="C27" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
         <v>83</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>84</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" t="s">
         <v>86</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>87</v>
-      </c>
-      <c r="C29" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
         <v>89</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>90</v>
-      </c>
-      <c r="C30" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" t="s">
         <v>92</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>93</v>
-      </c>
-      <c r="C31" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" t="s">
         <v>95</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>96</v>
-      </c>
-      <c r="C32" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" t="s">
         <v>98</v>
-      </c>
-      <c r="B33" t="s">
-        <v>102</v>
-      </c>
-      <c r="C33" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" t="s">
         <v>100</v>
-      </c>
-      <c r="B34" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" t="s">
         <v>104</v>
-      </c>
-      <c r="B35" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
         <v>106</v>
-      </c>
-      <c r="B36" t="s">
-        <v>110</v>
-      </c>
-      <c r="C36" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" t="s">
         <v>113</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>114</v>
-      </c>
-      <c r="C38" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="B40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B44" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C45" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B46" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C46" t="s">
         <v>30</v>
@@ -1319,10 +1319,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B47" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C47" t="s">
         <v>31</v>
@@ -1330,68 +1330,68 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B48" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C48" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B49" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B52" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C52" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for comoment macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="163">
   <si>
     <t>Test</t>
   </si>
@@ -490,6 +490,24 @@
   </si>
   <si>
     <t>Treynor_Ratio_test2</t>
+  </si>
+  <si>
+    <t>comoment_test1</t>
+  </si>
+  <si>
+    <t>Comoment1</t>
+  </si>
+  <si>
+    <t>Test coSkewness</t>
+  </si>
+  <si>
+    <t>Comoment2</t>
+  </si>
+  <si>
+    <t>Test coKurtosis</t>
+  </si>
+  <si>
+    <t>comoment_test2</t>
   </si>
 </sst>
 </file>
@@ -807,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1403,6 +1421,28 @@
         <v>156</v>
       </c>
     </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" t="s">
+        <v>159</v>
+      </c>
+      <c r="C54" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add tests to BetaCoMoments, TEST2 needs to be fixed
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="172">
   <si>
     <t>Test</t>
   </si>
@@ -508,6 +508,33 @@
   </si>
   <si>
     <t>comoment_test2</t>
+  </si>
+  <si>
+    <t>BetaCoMoments_test1</t>
+  </si>
+  <si>
+    <t>BetaCoMoments1</t>
+  </si>
+  <si>
+    <t>Test Beta Covariance</t>
+  </si>
+  <si>
+    <t>BetaCoMoments2</t>
+  </si>
+  <si>
+    <t>Test Beta Coskewness</t>
+  </si>
+  <si>
+    <t>BetaCoMoments3</t>
+  </si>
+  <si>
+    <t>Test Beta Cokurtosis</t>
+  </si>
+  <si>
+    <t>BetaCoMoments_test2</t>
+  </si>
+  <si>
+    <t>BetaCoMoments_test3</t>
   </si>
 </sst>
 </file>
@@ -825,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1443,6 +1470,39 @@
         <v>162</v>
       </c>
     </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>168</v>
+      </c>
+      <c r="B58" t="s">
+        <v>169</v>
+      </c>
+      <c r="C58" t="s">
+        <v>171</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Complete test for Systematic_Risk macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="175">
   <si>
     <t>Test</t>
   </si>
@@ -318,9 +318,6 @@
     <t>Systematic_Risk_test1</t>
   </si>
   <si>
-    <t>Test Systematic Risk</t>
-  </si>
-  <si>
     <t>Systematic Risk1</t>
   </si>
   <si>
@@ -535,6 +532,18 @@
   </si>
   <si>
     <t>BetaCoMoments_test3</t>
+  </si>
+  <si>
+    <t>Systematic Risk2</t>
+  </si>
+  <si>
+    <t>Test Systematic Risk with scale=252</t>
+  </si>
+  <si>
+    <t>Test Systematic Risk with scale=1</t>
+  </si>
+  <si>
+    <t>Systematic_Risk_test2</t>
   </si>
 </sst>
 </file>
@@ -844,7 +853,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -852,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -917,7 +926,7 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1079,7 +1088,7 @@
         <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C20" t="s">
         <v>77</v>
@@ -1153,90 +1162,90 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" t="s">
         <v>100</v>
       </c>
-      <c r="B27" t="s">
-        <v>99</v>
-      </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" t="s">
         <v>105</v>
       </c>
-      <c r="B31" t="s">
-        <v>106</v>
-      </c>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1247,7 +1256,7 @@
         <v>124</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1255,54 +1264,54 @@
         <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C37" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
         <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>138</v>
       </c>
       <c r="B40" t="s">
         <v>134</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1316,70 +1325,70 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>138</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="C45" t="s">
-        <v>142</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B46" t="s">
         <v>146</v>
       </c>
       <c r="C46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="B47" t="s">
         <v>147</v>
       </c>
       <c r="C47" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1390,59 +1399,59 @@
         <v>148</v>
       </c>
       <c r="C48" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B49" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C49" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="B50" t="s">
         <v>151</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B51" t="s">
         <v>152</v>
       </c>
       <c r="C51" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>153</v>
       </c>
       <c r="B52" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C52" t="s">
-        <v>97</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C53" t="s">
         <v>156</v>
@@ -1450,21 +1459,21 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B54" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C54" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B55" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C55" t="s">
         <v>162</v>
@@ -1472,21 +1481,21 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B56" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C56" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C57" t="s">
         <v>170</v>
@@ -1494,13 +1503,24 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>168</v>
+        <v>99</v>
       </c>
       <c r="B58" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>171</v>
+      </c>
+      <c r="B59" t="s">
+        <v>173</v>
+      </c>
+      <c r="C59" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for TrackingError macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="181">
   <si>
     <t>Test</t>
   </si>
@@ -544,6 +544,24 @@
   </si>
   <si>
     <t>Systematic_Risk_test2</t>
+  </si>
+  <si>
+    <t>TrackingError1</t>
+  </si>
+  <si>
+    <t>Test Tracking Error with scale=252</t>
+  </si>
+  <si>
+    <t>Tracking_Error_test1</t>
+  </si>
+  <si>
+    <t>TrackingError2</t>
+  </si>
+  <si>
+    <t>Test Tracking Error with scale=1</t>
+  </si>
+  <si>
+    <t>Tracking_Error_test2</t>
   </si>
 </sst>
 </file>
@@ -853,7 +871,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -861,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1523,6 +1541,28 @@
         <v>174</v>
       </c>
     </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>175</v>
+      </c>
+      <c r="B60" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>178</v>
+      </c>
+      <c r="B61" t="s">
+        <v>179</v>
+      </c>
+      <c r="C61" t="s">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Complete test for Information_Ratio macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="187">
   <si>
     <t>Test</t>
   </si>
@@ -562,6 +562,24 @@
   </si>
   <si>
     <t>Tracking_Error_test2</t>
+  </si>
+  <si>
+    <t>Information_Ratio1</t>
+  </si>
+  <si>
+    <t>Test Information Ratio with scale=252</t>
+  </si>
+  <si>
+    <t>Information_Ratio_test1</t>
+  </si>
+  <si>
+    <t>Information_Ratio2</t>
+  </si>
+  <si>
+    <t>Test Information Ratio with scale=1</t>
+  </si>
+  <si>
+    <t>Information_Ratio_test2</t>
   </si>
 </sst>
 </file>
@@ -871,7 +889,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -879,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1563,6 +1581,28 @@
         <v>180</v>
       </c>
     </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>181</v>
+      </c>
+      <c r="B62" t="s">
+        <v>182</v>
+      </c>
+      <c r="C62" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>184</v>
+      </c>
+      <c r="B63" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" t="s">
+        <v>186</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Complete test for Specific_Risk macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
   <si>
     <t>Test</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Table_SpecificRisk</t>
   </si>
   <si>
-    <t>Test Specific Risk</t>
-  </si>
-  <si>
     <t>table_SpecificRisk_test1</t>
   </si>
   <si>
@@ -580,6 +577,18 @@
   </si>
   <si>
     <t>Information_Ratio_test2</t>
+  </si>
+  <si>
+    <t>Specific_Risk</t>
+  </si>
+  <si>
+    <t>Test Specific Risk table with scale=252</t>
+  </si>
+  <si>
+    <t>Test Specific Risk with scale=252</t>
+  </si>
+  <si>
+    <t>Specific_Risk_test</t>
   </si>
 </sst>
 </file>
@@ -889,7 +898,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -897,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,7 +971,7 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1047,238 +1056,238 @@
         <v>53</v>
       </c>
       <c r="B13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" t="s">
         <v>54</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>57</v>
-      </c>
-      <c r="C14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
         <v>59</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>60</v>
-      </c>
-      <c r="C15" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="s">
         <v>67</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>68</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
         <v>70</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>71</v>
-      </c>
-      <c r="C18" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>74</v>
-      </c>
-      <c r="C19" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" t="s">
         <v>76</v>
-      </c>
-      <c r="B20" t="s">
-        <v>131</v>
-      </c>
-      <c r="C20" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>79</v>
-      </c>
-      <c r="C21" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
         <v>81</v>
-      </c>
-      <c r="B22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
         <v>83</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>84</v>
-      </c>
-      <c r="C23" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" t="s">
         <v>87</v>
-      </c>
-      <c r="B24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
         <v>89</v>
-      </c>
-      <c r="B25" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" t="s">
         <v>127</v>
-      </c>
-      <c r="B27" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
         <v>101</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>102</v>
-      </c>
-      <c r="C28" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
         <v>62</v>
-      </c>
-      <c r="C29" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" t="s">
         <v>104</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>105</v>
-      </c>
-      <c r="C30" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" t="s">
         <v>111</v>
-      </c>
-      <c r="B31" t="s">
-        <v>105</v>
-      </c>
-      <c r="C31" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
         <v>113</v>
-      </c>
-      <c r="B32" t="s">
-        <v>105</v>
-      </c>
-      <c r="C32" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" t="s">
         <v>115</v>
-      </c>
-      <c r="B33" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C34" t="s">
         <v>24</v>
@@ -1286,10 +1295,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C35" t="s">
         <v>25</v>
@@ -1297,24 +1306,24 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" t="s">
         <v>119</v>
-      </c>
-      <c r="B36" t="s">
-        <v>126</v>
-      </c>
-      <c r="C36" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" t="s">
         <v>121</v>
-      </c>
-      <c r="B37" t="s">
-        <v>125</v>
-      </c>
-      <c r="C37" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1322,7 +1331,7 @@
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
@@ -1333,7 +1342,7 @@
         <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
         <v>19</v>
@@ -1341,24 +1350,24 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -1385,13 +1394,13 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1399,7 +1408,7 @@
         <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C45" t="s">
         <v>21</v>
@@ -1410,7 +1419,7 @@
         <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C46" t="s">
         <v>23</v>
@@ -1418,32 +1427,32 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" t="s">
         <v>143</v>
-      </c>
-      <c r="B48" t="s">
-        <v>148</v>
-      </c>
-      <c r="C48" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" t="s">
         <v>149</v>
-      </c>
-      <c r="B49" t="s">
-        <v>150</v>
       </c>
       <c r="C49" t="s">
         <v>46</v>
@@ -1451,156 +1460,167 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" t="s">
         <v>109</v>
-      </c>
-      <c r="B50" t="s">
-        <v>151</v>
-      </c>
-      <c r="C50" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" t="s">
         <v>96</v>
-      </c>
-      <c r="B51" t="s">
-        <v>152</v>
-      </c>
-      <c r="C51" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52" t="s">
         <v>153</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>154</v>
-      </c>
-      <c r="C52" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" t="s">
         <v>157</v>
       </c>
-      <c r="B53" t="s">
-        <v>158</v>
-      </c>
       <c r="C53" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" t="s">
         <v>159</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>160</v>
-      </c>
-      <c r="C54" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" t="s">
         <v>163</v>
       </c>
-      <c r="B55" t="s">
-        <v>164</v>
-      </c>
       <c r="C55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" t="s">
         <v>165</v>
       </c>
-      <c r="B56" t="s">
-        <v>166</v>
-      </c>
       <c r="C56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" t="s">
         <v>167</v>
       </c>
-      <c r="B57" t="s">
-        <v>168</v>
-      </c>
       <c r="C57" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B58" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B59" t="s">
+        <v>172</v>
+      </c>
+      <c r="C59" t="s">
         <v>173</v>
-      </c>
-      <c r="C59" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>174</v>
+      </c>
+      <c r="B60" t="s">
         <v>175</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>176</v>
-      </c>
-      <c r="C60" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>177</v>
+      </c>
+      <c r="B61" t="s">
         <v>178</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>179</v>
-      </c>
-      <c r="C61" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>180</v>
+      </c>
+      <c r="B62" t="s">
         <v>181</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>182</v>
-      </c>
-      <c r="C62" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>183</v>
+      </c>
+      <c r="B63" t="s">
         <v>184</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>185</v>
       </c>
-      <c r="C63" t="s">
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>186</v>
+      </c>
+      <c r="B64" t="s">
+        <v>188</v>
+      </c>
+      <c r="C64" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for Geo_Mean macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="193">
   <si>
     <t>Test</t>
   </si>
@@ -589,6 +589,15 @@
   </si>
   <si>
     <t>Specific_Risk_test</t>
+  </si>
+  <si>
+    <t>geo_mean_test</t>
+  </si>
+  <si>
+    <t>Geo_Mean</t>
+  </si>
+  <si>
+    <t>Test geometric mean</t>
   </si>
 </sst>
 </file>
@@ -898,7 +907,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -906,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1623,6 +1632,17 @@
         <v>189</v>
       </c>
     </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>191</v>
+      </c>
+      <c r="B65" t="s">
+        <v>192</v>
+      </c>
+      <c r="C65" t="s">
+        <v>190</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Complete test to return_centered macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="196">
   <si>
     <t>Test</t>
   </si>
@@ -598,6 +598,15 @@
   </si>
   <si>
     <t>Test geometric mean</t>
+  </si>
+  <si>
+    <t>Return_centered</t>
+  </si>
+  <si>
+    <t>Test centered return</t>
+  </si>
+  <si>
+    <t>return_centered_test</t>
   </si>
 </sst>
 </file>
@@ -907,7 +916,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -915,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1643,6 +1652,17 @@
         <v>190</v>
       </c>
     </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>193</v>
+      </c>
+      <c r="B66" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Complete test for Appraisal_Ratio macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="202">
   <si>
     <t>Test</t>
   </si>
@@ -219,12 +219,6 @@
     <t>fama_beta_test1</t>
   </si>
   <si>
-    <t>appraisal ratio</t>
-  </si>
-  <si>
-    <t>Test appraisal ratio</t>
-  </si>
-  <si>
     <t>appraisal_ratio_test1</t>
   </si>
   <si>
@@ -607,6 +601,30 @@
   </si>
   <si>
     <t>return_centered_test</t>
+  </si>
+  <si>
+    <t>appraisal ratio1</t>
+  </si>
+  <si>
+    <t>appraisal ratio2</t>
+  </si>
+  <si>
+    <t>appraisal ratio3</t>
+  </si>
+  <si>
+    <t>Test appraisal ratio with option=appraisal</t>
+  </si>
+  <si>
+    <t>Test appraisal ratio with option=modified</t>
+  </si>
+  <si>
+    <t>Test appraisal ratio with option=alternative</t>
+  </si>
+  <si>
+    <t>appraisal_ratio_test2</t>
+  </si>
+  <si>
+    <t>appraisal_ratio_test3</t>
   </si>
 </sst>
 </file>
@@ -916,7 +934,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -924,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,7 +1007,7 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1074,7 +1092,7 @@
         <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C13" t="s">
         <v>54</v>
@@ -1115,32 +1133,32 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>128</v>
       </c>
       <c r="C19" t="s">
         <v>74</v>
@@ -1151,18 +1169,18 @@
         <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
         <v>79</v>
@@ -1173,21 +1191,21 @@
         <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1203,68 +1221,68 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
         <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
         <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1272,7 +1290,7 @@
         <v>110</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
         <v>111</v>
@@ -1294,32 +1312,32 @@
         <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B35" t="s">
         <v>123</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1327,186 +1345,186 @@
         <v>118</v>
       </c>
       <c r="B36" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C36" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C37" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" t="s">
         <v>131</v>
       </c>
-      <c r="C38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" t="s">
-        <v>132</v>
-      </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C40" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>136</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" t="s">
         <v>144</v>
       </c>
-      <c r="C45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>22</v>
-      </c>
-      <c r="B46" t="s">
-        <v>145</v>
-      </c>
       <c r="C46" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" t="s">
         <v>141</v>
-      </c>
-      <c r="B47" t="s">
-        <v>146</v>
-      </c>
-      <c r="C47" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B48" t="s">
         <v>147</v>
       </c>
       <c r="C48" t="s">
-        <v>143</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" t="s">
         <v>148</v>
       </c>
-      <c r="B49" t="s">
-        <v>149</v>
-      </c>
       <c r="C49" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="B51" t="s">
         <v>151</v>
       </c>
       <c r="C51" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B52" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" t="s">
         <v>153</v>
-      </c>
-      <c r="C52" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1517,18 +1535,18 @@
         <v>157</v>
       </c>
       <c r="C53" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B54" t="s">
+        <v>161</v>
+      </c>
+      <c r="C54" t="s">
         <v>159</v>
-      </c>
-      <c r="C54" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1539,7 +1557,7 @@
         <v>163</v>
       </c>
       <c r="C55" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1550,95 +1568,95 @@
         <v>165</v>
       </c>
       <c r="C56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C57" t="s">
-        <v>169</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>168</v>
       </c>
       <c r="B58" t="s">
+        <v>170</v>
+      </c>
+      <c r="C58" t="s">
         <v>171</v>
-      </c>
-      <c r="C58" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B59" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C59" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B60" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C60" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B61" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C61" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B62" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C62" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B63" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C63" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B64" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" t="s">
         <v>188</v>
-      </c>
-      <c r="C64" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1649,18 +1667,40 @@
         <v>192</v>
       </c>
       <c r="C65" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B66" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>195</v>
+      </c>
+      <c r="B67" t="s">
+        <v>198</v>
+      </c>
+      <c r="C67" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>196</v>
+      </c>
+      <c r="B68" t="s">
+        <v>199</v>
+      </c>
+      <c r="C68" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for MSquared macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="211">
   <si>
     <t>Test</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Test alpha and beta values</t>
   </si>
   <si>
-    <t>CAPM_epsilon</t>
-  </si>
-  <si>
     <t>Test error term</t>
   </si>
   <si>
@@ -231,12 +228,6 @@
     <t>CAPM_JensenAlpha_test1</t>
   </si>
   <si>
-    <t>Msquared</t>
-  </si>
-  <si>
-    <t>Test Msquared</t>
-  </si>
-  <si>
     <t>Msquared_test1</t>
   </si>
   <si>
@@ -625,16 +616,58 @@
   </si>
   <si>
     <t>appraisal_ratio_test3</t>
+  </si>
+  <si>
+    <t>CAPM_epsilon1</t>
+  </si>
+  <si>
+    <t>Test Msquared with method=discrete, scale=252</t>
+  </si>
+  <si>
+    <t>Msquared1</t>
+  </si>
+  <si>
+    <t>Msquared2</t>
+  </si>
+  <si>
+    <t>Test Msquared with method=discrete, scale=1</t>
+  </si>
+  <si>
+    <t>Msquared_test2</t>
+  </si>
+  <si>
+    <t>Msquared_test3</t>
+  </si>
+  <si>
+    <t>Msquared_test4</t>
+  </si>
+  <si>
+    <t>Test Msquared with method=log, scale=4</t>
+  </si>
+  <si>
+    <t>Test Msquared with method=log, scale=12</t>
+  </si>
+  <si>
+    <t>Msquared3</t>
+  </si>
+  <si>
+    <t>Msquared4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -660,8 +693,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -934,7 +968,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -942,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,755 +989,791 @@
     <col min="3" max="3" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>141</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>191</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>194</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>192</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>195</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>193</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>185</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>161</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>153</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>186</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>187</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>175</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>176</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>124</v>
+        <v>178</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>179</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>188</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="B36" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="B37" t="s">
         <v>129</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>16</v>
       </c>
       <c r="C39" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="C44" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="B47" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>181</v>
       </c>
       <c r="B49" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="C49" t="s">
-        <v>107</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C51" t="s">
-        <v>152</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="C52" t="s">
-        <v>153</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B53" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C53" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>160</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>55</v>
       </c>
       <c r="C54" t="s">
-        <v>159</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>95</v>
       </c>
       <c r="B55" t="s">
-        <v>163</v>
+        <v>96</v>
       </c>
       <c r="C55" t="s">
-        <v>166</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B56" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="C56" t="s">
-        <v>167</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="C57" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>168</v>
+        <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>170</v>
+        <v>47</v>
       </c>
       <c r="C58" t="s">
-        <v>171</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>172</v>
+        <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>173</v>
+        <v>50</v>
       </c>
       <c r="C59" t="s">
-        <v>174</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>175</v>
+        <v>52</v>
       </c>
       <c r="B60" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C60" t="s">
-        <v>177</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>178</v>
+        <v>39</v>
       </c>
       <c r="B61" t="s">
-        <v>179</v>
+        <v>40</v>
       </c>
       <c r="C61" t="s">
-        <v>180</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
       <c r="B62" t="s">
-        <v>182</v>
+        <v>43</v>
       </c>
       <c r="C62" t="s">
-        <v>183</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B63" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C63" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B64" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="C64" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>191</v>
+        <v>90</v>
       </c>
       <c r="B65" t="s">
-        <v>192</v>
+        <v>146</v>
       </c>
       <c r="C65" t="s">
-        <v>193</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>194</v>
+        <v>147</v>
       </c>
       <c r="B66" t="s">
-        <v>197</v>
+        <v>148</v>
       </c>
       <c r="C66" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>195</v>
+        <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>198</v>
+        <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>200</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B68" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C68" t="s">
-        <v>201</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>202</v>
+      </c>
+      <c r="B69" t="s">
+        <v>203</v>
+      </c>
+      <c r="C69" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>209</v>
+      </c>
+      <c r="B70" t="s">
+        <v>207</v>
+      </c>
+      <c r="C70" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>210</v>
+      </c>
+      <c r="B71" t="s">
+        <v>208</v>
+      </c>
+      <c r="C71" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:C68">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Complete test for table_Annualized_Returns macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="220">
   <si>
     <t>Test</t>
   </si>
@@ -99,12 +99,6 @@
     <t>SharpeRatio_annualized_test2</t>
   </si>
   <si>
-    <t>Annualized Returns Table</t>
-  </si>
-  <si>
-    <t>Test Annualized table</t>
-  </si>
-  <si>
     <t>table_Annualized_Returns_test1</t>
   </si>
   <si>
@@ -652,6 +646,39 @@
   </si>
   <si>
     <t>Msquared4</t>
+  </si>
+  <si>
+    <t>Table_Annualized Returns1</t>
+  </si>
+  <si>
+    <t>Table_Annualized Returns2</t>
+  </si>
+  <si>
+    <t>Table_Annualized Returns3</t>
+  </si>
+  <si>
+    <t>Table_Annualized Returns4</t>
+  </si>
+  <si>
+    <t>table_Annualized_Returns_test2</t>
+  </si>
+  <si>
+    <t>table_Annualized_Returns_test3</t>
+  </si>
+  <si>
+    <t>table_Annualized_Returns_test4</t>
+  </si>
+  <si>
+    <t>Test Annualized table with method=discrete, scale=252, digits=4</t>
+  </si>
+  <si>
+    <t>Test Annualized table with method=discrete, scale=1, digits=8</t>
+  </si>
+  <si>
+    <t>Test Annualized table with method=log, scale=4, digits=6</t>
+  </si>
+  <si>
+    <t>Test Annualized table with method=log, scale=12, digits=6</t>
   </si>
 </sst>
 </file>
@@ -968,7 +995,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -976,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,134 +1029,134 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
         <v>98</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
         <v>57</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" t="s">
         <v>136</v>
-      </c>
-      <c r="B8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>189</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>192</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>198</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1140,7 +1167,7 @@
         <v>158</v>
       </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1151,62 +1178,62 @@
         <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>164</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
         <v>121</v>
-      </c>
-      <c r="B17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>197</v>
+      </c>
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1217,84 +1244,84 @@
         <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>153</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>154</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>184</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>185</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C24" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C25" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>180</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1302,18 +1329,18 @@
         <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
         <v>74</v>
@@ -1324,109 +1351,109 @@
         <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>186</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>187</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>189</v>
+        <v>124</v>
       </c>
       <c r="C33" t="s">
-        <v>190</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="B35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>129</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>131</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>134</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>135</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1442,24 +1469,24 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
         <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1467,32 +1494,32 @@
         <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
         <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1500,7 +1527,7 @@
         <v>113</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C47" t="s">
         <v>114</v>
@@ -1508,131 +1535,131 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>179</v>
       </c>
       <c r="B48" t="s">
-        <v>119</v>
+        <v>181</v>
       </c>
       <c r="C48" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
       <c r="C49" t="s">
-        <v>184</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C50" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="C51" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>163</v>
       </c>
       <c r="B52" t="s">
+        <v>165</v>
+      </c>
+      <c r="C52" t="s">
         <v>166</v>
-      </c>
-      <c r="C52" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>167</v>
+        <v>53</v>
       </c>
       <c r="C53" t="s">
-        <v>168</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="C54" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>142</v>
       </c>
       <c r="C55" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" t="s">
         <v>143</v>
       </c>
-      <c r="B56" t="s">
-        <v>144</v>
-      </c>
       <c r="C56" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>145</v>
+        <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C58" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>180</v>
       </c>
       <c r="C59" t="s">
         <v>51</v>
@@ -1640,134 +1667,167 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B60" t="s">
-        <v>182</v>
+        <v>38</v>
       </c>
       <c r="C60" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C61" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>42</v>
+        <v>167</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>168</v>
       </c>
       <c r="C62" t="s">
-        <v>44</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B63" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C63" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>172</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="C64" t="s">
-        <v>174</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>90</v>
+        <v>145</v>
       </c>
       <c r="B65" t="s">
         <v>146</v>
       </c>
       <c r="C65" t="s">
-        <v>91</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>147</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
-        <v>148</v>
+        <v>61</v>
       </c>
       <c r="C66" t="s">
-        <v>149</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>199</v>
       </c>
       <c r="B67" t="s">
-        <v>63</v>
+        <v>198</v>
       </c>
       <c r="C67" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>200</v>
+      </c>
+      <c r="B68" t="s">
         <v>201</v>
       </c>
-      <c r="B68" t="s">
-        <v>200</v>
-      </c>
       <c r="C68" t="s">
-        <v>69</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B69" t="s">
+        <v>205</v>
+      </c>
+      <c r="C69" t="s">
         <v>203</v>
-      </c>
-      <c r="C69" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B70" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C70" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>209</v>
+      </c>
+      <c r="B71" t="s">
+        <v>216</v>
+      </c>
+      <c r="C71" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>210</v>
       </c>
-      <c r="B71" t="s">
-        <v>208</v>
-      </c>
-      <c r="C71" t="s">
-        <v>206</v>
+      <c r="B72" t="s">
+        <v>217</v>
+      </c>
+      <c r="C72" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>211</v>
+      </c>
+      <c r="B73" t="s">
+        <v>218</v>
+      </c>
+      <c r="C73" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>212</v>
+      </c>
+      <c r="B74" t="s">
+        <v>219</v>
+      </c>
+      <c r="C74" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for table_autocorrelation macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -123,15 +123,9 @@
     <t>table_correlation_test1</t>
   </si>
   <si>
-    <t>AutoCorrelation Table</t>
-  </si>
-  <si>
     <t>Test autocorrelation table</t>
   </si>
   <si>
-    <t>table_autocorrelation_test1</t>
-  </si>
-  <si>
     <t>Table_Stats</t>
   </si>
   <si>
@@ -679,6 +673,12 @@
   </si>
   <si>
     <t>Test Annualized table with method=log, scale=12, digits=6</t>
+  </si>
+  <si>
+    <t>Table_AutoCorrelation</t>
+  </si>
+  <si>
+    <t>table_autocorrelation_test</t>
   </si>
 </sst>
 </file>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,123 +1029,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
         <v>96</v>
-      </c>
-      <c r="B3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
         <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" t="s">
         <v>193</v>
-      </c>
-      <c r="C10" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" t="s">
         <v>194</v>
-      </c>
-      <c r="C11" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>154</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1156,7 +1156,7 @@
         <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1167,62 +1167,62 @@
         <v>158</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
         <v>119</v>
-      </c>
-      <c r="B16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C16" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>195</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>121</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>147</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>148</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1233,84 +1233,84 @@
         <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>153</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>182</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>183</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C23" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C24" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>178</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1318,18 +1318,18 @@
         <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>123</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
         <v>72</v>
@@ -1340,109 +1340,109 @@
         <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>184</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>185</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>186</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>187</v>
+        <v>122</v>
       </c>
       <c r="C32" t="s">
-        <v>188</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>133</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1458,24 +1458,24 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
         <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1483,32 +1483,32 @@
         <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B45" t="s">
         <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1516,7 +1516,7 @@
         <v>111</v>
       </c>
       <c r="B46" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
         <v>112</v>
@@ -1524,131 +1524,131 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
       <c r="C47" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>179</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>181</v>
+        <v>135</v>
       </c>
       <c r="C48" t="s">
-        <v>182</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C49" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="B51" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" t="s">
         <v>164</v>
-      </c>
-      <c r="C51" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>163</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>165</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>166</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="B54" t="s">
-        <v>94</v>
+        <v>140</v>
       </c>
       <c r="C54" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" t="s">
         <v>141</v>
       </c>
-      <c r="B55" t="s">
-        <v>142</v>
-      </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="B56" t="s">
-        <v>143</v>
+        <v>43</v>
       </c>
       <c r="C56" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="C58" t="s">
         <v>49</v>
@@ -1656,178 +1656,178 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B59" t="s">
-        <v>180</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C60" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>166</v>
       </c>
       <c r="C61" t="s">
-        <v>42</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B62" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C62" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>170</v>
+        <v>86</v>
       </c>
       <c r="B63" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="C63" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="B64" t="s">
         <v>144</v>
       </c>
       <c r="C64" t="s">
-        <v>89</v>
+        <v>145</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>145</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>146</v>
+        <v>59</v>
       </c>
       <c r="C65" t="s">
-        <v>147</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>197</v>
       </c>
       <c r="B66" t="s">
-        <v>61</v>
+        <v>196</v>
       </c>
       <c r="C66" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>198</v>
+      </c>
+      <c r="B67" t="s">
         <v>199</v>
       </c>
-      <c r="B67" t="s">
-        <v>198</v>
-      </c>
       <c r="C67" t="s">
-        <v>67</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B68" t="s">
+        <v>203</v>
+      </c>
+      <c r="C68" t="s">
         <v>201</v>
-      </c>
-      <c r="C68" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B69" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C69" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B70" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C70" t="s">
-        <v>204</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B71" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C71" t="s">
-        <v>26</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B72" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C72" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B73" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C73" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B74" t="s">
+        <v>34</v>
+      </c>
+      <c r="C74" t="s">
         <v>219</v>
-      </c>
-      <c r="C74" t="s">
-        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for table_CAPM macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="223">
   <si>
     <t>Test</t>
   </si>
@@ -297,9 +297,6 @@
     <t>table_CAPM1</t>
   </si>
   <si>
-    <t>Test CAPM table</t>
-  </si>
-  <si>
     <t>table_CAPM_test1</t>
   </si>
   <si>
@@ -679,6 +676,18 @@
   </si>
   <si>
     <t>table_autocorrelation_test</t>
+  </si>
+  <si>
+    <t>table_CAPM2</t>
+  </si>
+  <si>
+    <t>Test CAPM table with scale=252, digits=4</t>
+  </si>
+  <si>
+    <t>Test CAPM table with scale=1, digits=6</t>
+  </si>
+  <si>
+    <t>table_CAPM_test2</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1004,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1003,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,7 +1038,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>56</v>
@@ -1040,35 +1049,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
         <v>94</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>95</v>
-      </c>
-      <c r="C3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
         <v>101</v>
-      </c>
-      <c r="B4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
         <v>103</v>
-      </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1084,32 +1093,32 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" t="s">
         <v>133</v>
-      </c>
-      <c r="B8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C9" t="s">
         <v>61</v>
@@ -1117,68 +1126,68 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" t="s">
         <v>153</v>
       </c>
-      <c r="B12" t="s">
-        <v>154</v>
-      </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" t="s">
         <v>155</v>
       </c>
-      <c r="B13" t="s">
-        <v>156</v>
-      </c>
       <c r="C13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" t="s">
         <v>157</v>
       </c>
-      <c r="B14" t="s">
-        <v>158</v>
-      </c>
       <c r="C14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
         <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1189,12 +1198,12 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -1216,24 +1225,24 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19" t="s">
         <v>147</v>
       </c>
-      <c r="B19" t="s">
-        <v>148</v>
-      </c>
       <c r="C19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" t="s">
         <v>149</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>150</v>
-      </c>
-      <c r="C20" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1249,35 +1258,35 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" t="s">
         <v>182</v>
       </c>
-      <c r="B22" t="s">
-        <v>183</v>
-      </c>
       <c r="C22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" t="s">
         <v>171</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>172</v>
-      </c>
-      <c r="C23" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" t="s">
         <v>174</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>175</v>
-      </c>
-      <c r="C24" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1307,7 +1316,7 @@
         <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C27" t="s">
         <v>67</v>
@@ -1348,13 +1357,13 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>183</v>
+      </c>
+      <c r="B31" t="s">
         <v>184</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>185</v>
-      </c>
-      <c r="C31" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1362,7 +1371,7 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C32" t="s">
         <v>14</v>
@@ -1373,7 +1382,7 @@
         <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C33" t="s">
         <v>19</v>
@@ -1381,24 +1390,24 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1425,13 +1434,13 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1469,21 +1478,21 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" t="s">
         <v>105</v>
-      </c>
-      <c r="B42" t="s">
-        <v>97</v>
-      </c>
-      <c r="C42" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C43" t="s">
         <v>24</v>
@@ -1491,10 +1500,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
@@ -1502,35 +1511,35 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" t="s">
         <v>109</v>
-      </c>
-      <c r="B45" t="s">
-        <v>116</v>
-      </c>
-      <c r="C45" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" t="s">
         <v>111</v>
-      </c>
-      <c r="B46" t="s">
-        <v>115</v>
-      </c>
-      <c r="C46" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B47" t="s">
+        <v>178</v>
+      </c>
+      <c r="C47" t="s">
         <v>179</v>
-      </c>
-      <c r="C47" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1538,7 +1547,7 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C48" t="s">
         <v>21</v>
@@ -1549,7 +1558,7 @@
         <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C49" t="s">
         <v>23</v>
@@ -1560,7 +1569,7 @@
         <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
         <v>88</v>
@@ -1568,13 +1577,13 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" t="s">
         <v>163</v>
-      </c>
-      <c r="C51" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1590,145 +1599,145 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
       <c r="B54" t="s">
         <v>140</v>
       </c>
       <c r="C54" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="B55" t="s">
-        <v>141</v>
+        <v>43</v>
       </c>
       <c r="C55" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C56" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
       <c r="C57" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B58" t="s">
-        <v>178</v>
+        <v>36</v>
       </c>
       <c r="C58" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B59" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>38</v>
+        <v>164</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>165</v>
       </c>
       <c r="C60" t="s">
-        <v>40</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B61" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C61" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>168</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="C62" t="s">
-        <v>170</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="B63" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C63" t="s">
-        <v>87</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>143</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>145</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>196</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>195</v>
       </c>
       <c r="C65" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1736,18 +1745,18 @@
         <v>197</v>
       </c>
       <c r="B66" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C66" t="s">
-        <v>65</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B67" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C67" t="s">
         <v>200</v>
@@ -1769,10 +1778,10 @@
         <v>206</v>
       </c>
       <c r="B69" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="C69" t="s">
-        <v>202</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1783,7 +1792,7 @@
         <v>214</v>
       </c>
       <c r="C70" t="s">
-        <v>26</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1810,24 +1819,35 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="B73" t="s">
-        <v>217</v>
+        <v>34</v>
       </c>
       <c r="C73" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>218</v>
+        <v>91</v>
       </c>
       <c r="B74" t="s">
-        <v>34</v>
+        <v>220</v>
       </c>
       <c r="C74" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>219</v>
+      </c>
+      <c r="B75" t="s">
+        <v>221</v>
+      </c>
+      <c r="C75" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for table_InformationRatio macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -156,12 +156,6 @@
     <t>table_HigherMoments_test1</t>
   </si>
   <si>
-    <t>Table_InformationRatio</t>
-  </si>
-  <si>
-    <t>Test Information Ratio Table</t>
-  </si>
-  <si>
     <t>table_InformationRatio_test1</t>
   </si>
   <si>
@@ -688,6 +682,12 @@
   </si>
   <si>
     <t>table_CAPM_test2</t>
+  </si>
+  <si>
+    <t>Table_InformationRatio1</t>
+  </si>
+  <si>
+    <t>Test Information Ratio Table with scale=252</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1004,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1014,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,156 +1038,156 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
         <v>93</v>
-      </c>
-      <c r="B3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
         <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" t="s">
         <v>190</v>
-      </c>
-      <c r="C10" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" t="s">
         <v>191</v>
-      </c>
-      <c r="C11" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" t="s">
         <v>157</v>
-      </c>
-      <c r="C14" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1198,12 +1198,12 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -1214,35 +1214,35 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
         <v>62</v>
-      </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" t="s">
         <v>148</v>
-      </c>
-      <c r="B20" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1258,35 +1258,35 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B22" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" t="s">
         <v>170</v>
-      </c>
-      <c r="B23" t="s">
-        <v>171</v>
-      </c>
-      <c r="C23" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B24" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" t="s">
         <v>173</v>
-      </c>
-      <c r="B24" t="s">
-        <v>174</v>
-      </c>
-      <c r="C24" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1313,57 +1313,57 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
         <v>68</v>
-      </c>
-      <c r="B28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" t="s">
         <v>73</v>
-      </c>
-      <c r="B30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" t="s">
+        <v>182</v>
+      </c>
+      <c r="C31" t="s">
         <v>183</v>
-      </c>
-      <c r="B31" t="s">
-        <v>184</v>
-      </c>
-      <c r="C31" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1371,7 +1371,7 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C32" t="s">
         <v>14</v>
@@ -1382,7 +1382,7 @@
         <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
         <v>19</v>
@@ -1390,24 +1390,24 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B34" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" t="s">
         <v>123</v>
-      </c>
-      <c r="C34" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" t="s">
         <v>124</v>
-      </c>
-      <c r="C35" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1434,65 +1434,65 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
         <v>82</v>
-      </c>
-      <c r="B41" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
         <v>24</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
@@ -1511,35 +1511,35 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C46" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>174</v>
+      </c>
+      <c r="B47" t="s">
         <v>176</v>
       </c>
-      <c r="B47" t="s">
-        <v>178</v>
-      </c>
       <c r="C47" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1547,7 +1547,7 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C48" t="s">
         <v>21</v>
@@ -1558,7 +1558,7 @@
         <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C49" t="s">
         <v>23</v>
@@ -1566,186 +1566,186 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" t="s">
         <v>160</v>
       </c>
-      <c r="B51" t="s">
-        <v>162</v>
-      </c>
       <c r="C51" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>136</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>137</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" t="s">
         <v>138</v>
       </c>
-      <c r="B53" t="s">
-        <v>139</v>
-      </c>
       <c r="C53" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="B54" t="s">
-        <v>140</v>
+        <v>43</v>
       </c>
       <c r="C54" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>175</v>
       </c>
       <c r="C55" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C56" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B57" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="C57" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>162</v>
       </c>
       <c r="B58" t="s">
-        <v>36</v>
+        <v>163</v>
       </c>
       <c r="C58" t="s">
-        <v>37</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>165</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>166</v>
       </c>
       <c r="C59" t="s">
-        <v>40</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>164</v>
+        <v>84</v>
       </c>
       <c r="B60" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="C60" t="s">
-        <v>166</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="B61" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="C61" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>141</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>142</v>
+        <v>194</v>
       </c>
       <c r="B63" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="C63" t="s">
-        <v>144</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>195</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="C64" t="s">
-        <v>60</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C65" t="s">
-        <v>65</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B66" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C66" t="s">
         <v>199</v>
@@ -1756,10 +1756,10 @@
         <v>204</v>
       </c>
       <c r="B67" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C67" t="s">
-        <v>200</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1767,10 +1767,10 @@
         <v>205</v>
       </c>
       <c r="B68" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="C68" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1781,7 +1781,7 @@
         <v>213</v>
       </c>
       <c r="C69" t="s">
-        <v>26</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1797,24 +1797,24 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="B71" t="s">
-        <v>215</v>
+        <v>34</v>
       </c>
       <c r="C71" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>209</v>
+        <v>89</v>
       </c>
       <c r="B72" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C72" t="s">
-        <v>212</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1822,32 +1822,32 @@
         <v>217</v>
       </c>
       <c r="B73" t="s">
-        <v>34</v>
+        <v>219</v>
       </c>
       <c r="C73" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="B74" t="s">
-        <v>220</v>
+        <v>49</v>
       </c>
       <c r="C74" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B75" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C75" t="s">
-        <v>222</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for table_stats macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -132,9 +132,6 @@
     <t>Test stats table</t>
   </si>
   <si>
-    <t>table_stats_test1</t>
-  </si>
-  <si>
     <t>Table_variability</t>
   </si>
   <si>
@@ -688,6 +685,9 @@
   </si>
   <si>
     <t>Test Information Ratio Table with scale=252</t>
+  </si>
+  <si>
+    <t>table_stats_test</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,156 +1038,156 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
         <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
         <v>91</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>92</v>
-      </c>
-      <c r="C3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
         <v>98</v>
-      </c>
-      <c r="B4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
         <v>100</v>
-      </c>
-      <c r="B5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>52</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" t="s">
         <v>130</v>
-      </c>
-      <c r="B8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" t="s">
         <v>150</v>
       </c>
-      <c r="B12" t="s">
-        <v>151</v>
-      </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" t="s">
         <v>152</v>
       </c>
-      <c r="B13" t="s">
-        <v>153</v>
-      </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" t="s">
         <v>154</v>
       </c>
-      <c r="B14" t="s">
-        <v>155</v>
-      </c>
       <c r="C14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" t="s">
         <v>114</v>
-      </c>
-      <c r="B15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1198,12 +1198,12 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -1214,35 +1214,35 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
         <v>60</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>61</v>
-      </c>
-      <c r="C18" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" t="s">
         <v>144</v>
       </c>
-      <c r="B19" t="s">
-        <v>145</v>
-      </c>
       <c r="C19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" t="s">
         <v>146</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>147</v>
-      </c>
-      <c r="C20" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1258,35 +1258,35 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" t="s">
         <v>179</v>
       </c>
-      <c r="B22" t="s">
-        <v>180</v>
-      </c>
       <c r="C22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B23" t="s">
         <v>168</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>169</v>
-      </c>
-      <c r="C23" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" t="s">
         <v>171</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>172</v>
-      </c>
-      <c r="C24" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1313,57 +1313,57 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" t="s">
         <v>64</v>
-      </c>
-      <c r="B27" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
         <v>66</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>67</v>
-      </c>
-      <c r="C28" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" t="s">
         <v>69</v>
-      </c>
-      <c r="B29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
         <v>71</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>72</v>
-      </c>
-      <c r="C30" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>180</v>
+      </c>
+      <c r="B31" t="s">
         <v>181</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>182</v>
-      </c>
-      <c r="C31" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1371,7 +1371,7 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C32" t="s">
         <v>14</v>
@@ -1382,7 +1382,7 @@
         <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C33" t="s">
         <v>19</v>
@@ -1390,24 +1390,24 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1434,65 +1434,65 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
         <v>75</v>
-      </c>
-      <c r="B39" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" t="s">
         <v>77</v>
-      </c>
-      <c r="B40" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" t="s">
         <v>102</v>
-      </c>
-      <c r="B42" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C43" t="s">
         <v>24</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
@@ -1511,35 +1511,35 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" t="s">
         <v>106</v>
-      </c>
-      <c r="B45" t="s">
-        <v>113</v>
-      </c>
-      <c r="C45" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" t="s">
         <v>108</v>
-      </c>
-      <c r="B46" t="s">
-        <v>112</v>
-      </c>
-      <c r="C46" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B47" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" t="s">
         <v>176</v>
-      </c>
-      <c r="C47" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1547,7 +1547,7 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C48" t="s">
         <v>21</v>
@@ -1558,7 +1558,7 @@
         <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C49" t="s">
         <v>23</v>
@@ -1566,145 +1566,145 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B51" t="s">
+        <v>159</v>
+      </c>
+      <c r="C51" t="s">
         <v>160</v>
-      </c>
-      <c r="C51" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52" t="s">
         <v>136</v>
       </c>
-      <c r="B52" t="s">
-        <v>137</v>
-      </c>
       <c r="C52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" t="s">
         <v>96</v>
-      </c>
-      <c r="B53" t="s">
-        <v>138</v>
-      </c>
-      <c r="C53" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" t="s">
         <v>42</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>43</v>
-      </c>
-      <c r="C54" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" t="s">
+        <v>174</v>
+      </c>
+      <c r="C55" t="s">
         <v>46</v>
-      </c>
-      <c r="B55" t="s">
-        <v>175</v>
-      </c>
-      <c r="C55" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B56" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C56" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>38</v>
+        <v>161</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>162</v>
       </c>
       <c r="C57" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B58" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C58" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="B59" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="C59" t="s">
-        <v>167</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="B60" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C60" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>140</v>
+        <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>141</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>142</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>193</v>
       </c>
       <c r="B62" t="s">
-        <v>57</v>
+        <v>192</v>
       </c>
       <c r="C62" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1712,18 +1712,18 @@
         <v>194</v>
       </c>
       <c r="B63" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C63" t="s">
-        <v>63</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B64" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C64" t="s">
         <v>197</v>
@@ -1745,10 +1745,10 @@
         <v>203</v>
       </c>
       <c r="B66" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="C66" t="s">
-        <v>199</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1759,7 +1759,7 @@
         <v>211</v>
       </c>
       <c r="C67" t="s">
-        <v>26</v>
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1786,68 +1786,68 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="B70" t="s">
-        <v>214</v>
+        <v>34</v>
       </c>
       <c r="C70" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>215</v>
+        <v>88</v>
       </c>
       <c r="B71" t="s">
-        <v>34</v>
+        <v>217</v>
       </c>
       <c r="C71" t="s">
-        <v>216</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>216</v>
       </c>
       <c r="B72" t="s">
         <v>218</v>
       </c>
       <c r="C72" t="s">
-        <v>90</v>
+        <v>219</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>217</v>
+        <v>47</v>
       </c>
       <c r="B73" t="s">
-        <v>219</v>
+        <v>48</v>
       </c>
       <c r="C73" t="s">
-        <v>220</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>48</v>
+        <v>220</v>
       </c>
       <c r="B74" t="s">
-        <v>49</v>
+        <v>221</v>
       </c>
       <c r="C74" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>221</v>
+        <v>35</v>
       </c>
       <c r="B75" t="s">
+        <v>36</v>
+      </c>
+      <c r="C75" t="s">
         <v>222</v>
-      </c>
-      <c r="C75" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for table_correlation macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -114,15 +114,9 @@
     <t>CAPM_epsilon_test1</t>
   </si>
   <si>
-    <t>Correlation Table</t>
-  </si>
-  <si>
     <t>Test correlation table</t>
   </si>
   <si>
-    <t>table_correlation_test1</t>
-  </si>
-  <si>
     <t>Test autocorrelation table</t>
   </si>
   <si>
@@ -688,6 +682,12 @@
   </si>
   <si>
     <t>table_stats_test</t>
+  </si>
+  <si>
+    <t>Table_Correlation</t>
+  </si>
+  <si>
+    <t>table_correlation_test</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1004,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1014,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
       <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
@@ -1038,156 +1038,156 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
         <v>90</v>
-      </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
         <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" t="s">
         <v>187</v>
-      </c>
-      <c r="C10" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" t="s">
         <v>188</v>
-      </c>
-      <c r="C11" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" t="s">
         <v>154</v>
-      </c>
-      <c r="C14" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1198,12 +1198,12 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -1214,101 +1214,101 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
         <v>59</v>
-      </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" t="s">
         <v>145</v>
-      </c>
-      <c r="B20" t="s">
-        <v>146</v>
-      </c>
-      <c r="C20" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>176</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>177</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="C22" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B23" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>172</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1316,18 +1316,18 @@
         <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
         <v>67</v>
@@ -1338,109 +1338,109 @@
         <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>178</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>179</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>180</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>181</v>
+        <v>116</v>
       </c>
       <c r="C31" t="s">
-        <v>182</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>123</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
-        <v>127</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1456,24 +1456,24 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
         <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1481,32 +1481,32 @@
         <v>101</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44" t="s">
         <v>110</v>
       </c>
       <c r="C44" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1514,7 +1514,7 @@
         <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C45" t="s">
         <v>106</v>
@@ -1522,329 +1522,329 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
+        <v>173</v>
       </c>
       <c r="C46" t="s">
-        <v>108</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>173</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="C47" t="s">
-        <v>176</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C48" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="C49" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="B50" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" t="s">
         <v>158</v>
-      </c>
-      <c r="C50" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="B51" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="C51" t="s">
-        <v>160</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>93</v>
+      </c>
+      <c r="B52" t="s">
         <v>135</v>
       </c>
-      <c r="B52" t="s">
-        <v>136</v>
-      </c>
       <c r="C52" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>174</v>
+        <v>36</v>
       </c>
       <c r="C55" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>37</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
-        <v>38</v>
+        <v>160</v>
       </c>
       <c r="C56" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B57" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C57" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>164</v>
+        <v>81</v>
       </c>
       <c r="B58" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="C58" t="s">
-        <v>166</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="B59" t="s">
         <v>138</v>
       </c>
       <c r="C59" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>140</v>
+        <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>141</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>191</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>190</v>
       </c>
       <c r="C61" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" t="s">
         <v>193</v>
       </c>
-      <c r="B62" t="s">
-        <v>192</v>
-      </c>
       <c r="C62" t="s">
-        <v>62</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B63" t="s">
+        <v>197</v>
+      </c>
+      <c r="C63" t="s">
         <v>195</v>
-      </c>
-      <c r="C63" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B65" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C65" t="s">
-        <v>198</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C66" t="s">
-        <v>26</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C67" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B68" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C68" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B69" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" t="s">
         <v>213</v>
-      </c>
-      <c r="C69" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>214</v>
+        <v>86</v>
       </c>
       <c r="B70" t="s">
-        <v>34</v>
+        <v>215</v>
       </c>
       <c r="C70" t="s">
-        <v>215</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>214</v>
       </c>
       <c r="B71" t="s">
+        <v>216</v>
+      </c>
+      <c r="C71" t="s">
         <v>217</v>
-      </c>
-      <c r="C71" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>216</v>
+        <v>45</v>
       </c>
       <c r="B72" t="s">
-        <v>218</v>
+        <v>46</v>
       </c>
       <c r="C72" t="s">
-        <v>219</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>47</v>
+        <v>218</v>
       </c>
       <c r="B73" t="s">
-        <v>48</v>
+        <v>219</v>
       </c>
       <c r="C73" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>33</v>
+      </c>
+      <c r="B74" t="s">
+        <v>34</v>
+      </c>
+      <c r="C74" t="s">
         <v>220</v>
-      </c>
-      <c r="B74" t="s">
-        <v>221</v>
-      </c>
-      <c r="C74" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>35</v>
+        <v>221</v>
       </c>
       <c r="B75" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C75" t="s">
         <v>222</v>

</xml_diff>

<commit_message>
Complete test for table_CalendarReturns macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="226">
   <si>
     <t>Test</t>
   </si>
@@ -156,12 +156,6 @@
     <t>table_SpecificRisk_test1</t>
   </si>
   <si>
-    <t>Table_CalendarReturns</t>
-  </si>
-  <si>
-    <t>Test Calendar Returns</t>
-  </si>
-  <si>
     <t>table_CalendarReturns_test1</t>
   </si>
   <si>
@@ -688,6 +682,21 @@
   </si>
   <si>
     <t>table_correlation_test</t>
+  </si>
+  <si>
+    <t>Table_CalendarReturns1</t>
+  </si>
+  <si>
+    <t>Test Calendar Returns for simple returns with digits=6</t>
+  </si>
+  <si>
+    <t>Test Calendar Returns for compound returns with digits=8</t>
+  </si>
+  <si>
+    <t>Table_CalendarReturns2</t>
+  </si>
+  <si>
+    <t>table_CalendarReturns_test2</t>
   </si>
 </sst>
 </file>
@@ -1012,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,156 +1047,156 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
         <v>88</v>
-      </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
         <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" t="s">
         <v>185</v>
-      </c>
-      <c r="C10" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" t="s">
         <v>186</v>
-      </c>
-      <c r="C11" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" t="s">
         <v>152</v>
-      </c>
-      <c r="C14" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1198,12 +1207,12 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -1214,68 +1223,68 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
         <v>57</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" t="s">
         <v>143</v>
-      </c>
-      <c r="B20" t="s">
-        <v>144</v>
-      </c>
-      <c r="C20" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" t="s">
         <v>165</v>
-      </c>
-      <c r="B22" t="s">
-        <v>166</v>
-      </c>
-      <c r="C22" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" t="s">
         <v>168</v>
-      </c>
-      <c r="B23" t="s">
-        <v>169</v>
-      </c>
-      <c r="C23" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1302,57 +1311,57 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
         <v>63</v>
-      </c>
-      <c r="B27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
         <v>68</v>
-      </c>
-      <c r="B29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>176</v>
+      </c>
+      <c r="B30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" t="s">
         <v>178</v>
-      </c>
-      <c r="B30" t="s">
-        <v>179</v>
-      </c>
-      <c r="C30" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1360,7 +1369,7 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
@@ -1371,7 +1380,7 @@
         <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
         <v>19</v>
@@ -1379,24 +1388,24 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" t="s">
         <v>118</v>
-      </c>
-      <c r="C33" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" t="s">
         <v>119</v>
-      </c>
-      <c r="C34" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1423,65 +1432,65 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" t="s">
         <v>77</v>
-      </c>
-      <c r="B40" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C42" t="s">
         <v>24</v>
@@ -1489,10 +1498,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C43" t="s">
         <v>25</v>
@@ -1500,35 +1509,35 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>169</v>
+      </c>
+      <c r="B46" t="s">
         <v>171</v>
       </c>
-      <c r="B46" t="s">
-        <v>173</v>
-      </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1536,7 +1545,7 @@
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C47" t="s">
         <v>21</v>
@@ -1547,7 +1556,7 @@
         <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C48" t="s">
         <v>23</v>
@@ -1555,32 +1564,32 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B49" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" t="s">
         <v>155</v>
       </c>
-      <c r="B50" t="s">
-        <v>157</v>
-      </c>
       <c r="C50" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B51" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C51" t="s">
         <v>38</v>
@@ -1588,13 +1597,13 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C52" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1613,7 +1622,7 @@
         <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C54" t="s">
         <v>44</v>
@@ -1632,109 +1641,109 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>157</v>
+      </c>
+      <c r="B56" t="s">
+        <v>158</v>
+      </c>
+      <c r="C56" t="s">
         <v>159</v>
-      </c>
-      <c r="B56" t="s">
-        <v>160</v>
-      </c>
-      <c r="C56" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>160</v>
+      </c>
+      <c r="B57" t="s">
+        <v>161</v>
+      </c>
+      <c r="C57" t="s">
         <v>162</v>
-      </c>
-      <c r="B57" t="s">
-        <v>163</v>
-      </c>
-      <c r="C57" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C58" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>135</v>
+      </c>
+      <c r="B59" t="s">
+        <v>136</v>
+      </c>
+      <c r="C59" t="s">
         <v>137</v>
-      </c>
-      <c r="B59" t="s">
-        <v>138</v>
-      </c>
-      <c r="C59" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" t="s">
         <v>53</v>
-      </c>
-      <c r="B60" t="s">
-        <v>54</v>
-      </c>
-      <c r="C60" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B61" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C61" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>190</v>
+      </c>
+      <c r="B62" t="s">
+        <v>191</v>
+      </c>
+      <c r="C62" t="s">
         <v>192</v>
-      </c>
-      <c r="B62" t="s">
-        <v>193</v>
-      </c>
-      <c r="C62" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B63" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C63" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B64" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C64" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B65" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C65" t="s">
         <v>26</v>
@@ -1742,98 +1751,98 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B66" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C66" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B67" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C67" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B68" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C68" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B69" t="s">
         <v>32</v>
       </c>
       <c r="C69" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C70" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>212</v>
+      </c>
+      <c r="B71" t="s">
         <v>214</v>
       </c>
-      <c r="B71" t="s">
-        <v>216</v>
-      </c>
       <c r="C71" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>45</v>
+        <v>216</v>
       </c>
       <c r="B72" t="s">
-        <v>46</v>
+        <v>217</v>
       </c>
       <c r="C72" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" t="s">
+        <v>34</v>
+      </c>
+      <c r="C73" t="s">
         <v>218</v>
-      </c>
-      <c r="B73" t="s">
-        <v>219</v>
-      </c>
-      <c r="C73" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>33</v>
+        <v>219</v>
       </c>
       <c r="B74" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C74" t="s">
         <v>220</v>
@@ -1844,10 +1853,21 @@
         <v>221</v>
       </c>
       <c r="B75" t="s">
-        <v>31</v>
+        <v>222</v>
       </c>
       <c r="C75" t="s">
-        <v>222</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>224</v>
+      </c>
+      <c r="B76" t="s">
+        <v>223</v>
+      </c>
+      <c r="C76" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for table_HigherMoments macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -144,9 +144,6 @@
     <t>Test Higher Moments table</t>
   </si>
   <si>
-    <t>table_HigherMoments_test1</t>
-  </si>
-  <si>
     <t>table_InformationRatio_test1</t>
   </si>
   <si>
@@ -697,6 +694,9 @@
   </si>
   <si>
     <t>table_CalendarReturns_test2</t>
+  </si>
+  <si>
+    <t>table_HigherMoments_test</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,156 +1047,156 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
         <v>86</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>87</v>
-      </c>
-      <c r="C3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
         <v>93</v>
-      </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
         <v>95</v>
-      </c>
-      <c r="B5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
         <v>125</v>
-      </c>
-      <c r="B8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" t="s">
         <v>145</v>
       </c>
-      <c r="B12" t="s">
-        <v>146</v>
-      </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" t="s">
         <v>147</v>
       </c>
-      <c r="B13" t="s">
-        <v>148</v>
-      </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
         <v>149</v>
       </c>
-      <c r="B14" t="s">
-        <v>150</v>
-      </c>
       <c r="C14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
         <v>109</v>
-      </c>
-      <c r="B15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1207,12 +1207,12 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -1223,68 +1223,68 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
         <v>55</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>56</v>
-      </c>
-      <c r="C18" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" t="s">
         <v>139</v>
       </c>
-      <c r="B19" t="s">
-        <v>140</v>
-      </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" t="s">
         <v>141</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>142</v>
-      </c>
-      <c r="C20" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" t="s">
         <v>174</v>
       </c>
-      <c r="B21" t="s">
-        <v>175</v>
-      </c>
       <c r="C21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" t="s">
         <v>163</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>164</v>
-      </c>
-      <c r="C22" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" t="s">
         <v>166</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>167</v>
-      </c>
-      <c r="C23" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1311,57 +1311,57 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" t="s">
         <v>59</v>
-      </c>
-      <c r="B26" t="s">
-        <v>113</v>
-      </c>
-      <c r="C26" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
         <v>61</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>62</v>
-      </c>
-      <c r="C27" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
         <v>66</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>67</v>
-      </c>
-      <c r="C29" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" t="s">
         <v>176</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>177</v>
-      </c>
-      <c r="C30" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1369,7 +1369,7 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
@@ -1380,7 +1380,7 @@
         <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C32" t="s">
         <v>19</v>
@@ -1388,24 +1388,24 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1432,65 +1432,65 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" t="s">
         <v>70</v>
-      </c>
-      <c r="B38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" t="s">
         <v>72</v>
-      </c>
-      <c r="B39" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
         <v>97</v>
-      </c>
-      <c r="B41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
         <v>24</v>
@@ -1498,10 +1498,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C43" t="s">
         <v>25</v>
@@ -1509,35 +1509,35 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" t="s">
         <v>101</v>
-      </c>
-      <c r="B44" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" t="s">
         <v>103</v>
-      </c>
-      <c r="B45" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B46" t="s">
+        <v>170</v>
+      </c>
+      <c r="C46" t="s">
         <v>171</v>
-      </c>
-      <c r="C46" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1545,7 +1545,7 @@
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C47" t="s">
         <v>21</v>
@@ -1556,7 +1556,7 @@
         <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C48" t="s">
         <v>23</v>
@@ -1564,32 +1564,32 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B50" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" t="s">
         <v>155</v>
-      </c>
-      <c r="C50" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>130</v>
+      </c>
+      <c r="B51" t="s">
         <v>131</v>
-      </c>
-      <c r="B51" t="s">
-        <v>132</v>
       </c>
       <c r="C51" t="s">
         <v>38</v>
@@ -1597,101 +1597,101 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" t="s">
         <v>91</v>
-      </c>
-      <c r="B52" t="s">
-        <v>133</v>
-      </c>
-      <c r="C52" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
+        <v>169</v>
       </c>
       <c r="C53" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>170</v>
+        <v>36</v>
       </c>
       <c r="C54" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="C55" t="s">
-        <v>37</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C56" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>160</v>
+        <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="C57" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="B58" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>135</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>136</v>
+        <v>51</v>
       </c>
       <c r="C59" t="s">
-        <v>137</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>188</v>
       </c>
       <c r="B60" t="s">
-        <v>52</v>
+        <v>187</v>
       </c>
       <c r="C60" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1699,18 +1699,18 @@
         <v>189</v>
       </c>
       <c r="B61" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C61" t="s">
-        <v>58</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B62" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C62" t="s">
         <v>192</v>
@@ -1732,10 +1732,10 @@
         <v>198</v>
       </c>
       <c r="B64" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="C64" t="s">
-        <v>194</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1746,7 +1746,7 @@
         <v>206</v>
       </c>
       <c r="C65" t="s">
-        <v>26</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1773,98 +1773,98 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="B68" t="s">
-        <v>209</v>
+        <v>32</v>
       </c>
       <c r="C68" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>210</v>
+        <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>212</v>
       </c>
       <c r="C69" t="s">
-        <v>211</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>211</v>
       </c>
       <c r="B70" t="s">
         <v>213</v>
       </c>
       <c r="C70" t="s">
-        <v>85</v>
+        <v>214</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B71" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C71" t="s">
-        <v>215</v>
+        <v>41</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>216</v>
+        <v>33</v>
       </c>
       <c r="B72" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" t="s">
         <v>217</v>
-      </c>
-      <c r="C72" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>33</v>
+        <v>218</v>
       </c>
       <c r="B73" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C73" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B74" t="s">
-        <v>31</v>
+        <v>221</v>
       </c>
       <c r="C74" t="s">
-        <v>220</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B75" t="s">
         <v>222</v>
       </c>
       <c r="C75" t="s">
-        <v>45</v>
+        <v>224</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>224</v>
+        <v>39</v>
       </c>
       <c r="B76" t="s">
-        <v>223</v>
+        <v>40</v>
       </c>
       <c r="C76" t="s">
         <v>225</v>

</xml_diff>

<commit_message>
Create Mean_Abs_Deviation macro and add test for it
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="229">
   <si>
     <t>Test</t>
   </si>
@@ -697,6 +697,15 @@
   </si>
   <si>
     <t>table_HigherMoments_test</t>
+  </si>
+  <si>
+    <t>Mean_Abs_Deviation_test</t>
+  </si>
+  <si>
+    <t>Mean_Abs_Deviation</t>
+  </si>
+  <si>
+    <t>Test Mean Absolute Deviation</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1022,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1021,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1870,6 +1879,17 @@
         <v>225</v>
       </c>
     </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>227</v>
+      </c>
+      <c r="B77" t="s">
+        <v>228</v>
+      </c>
+      <c r="C77" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:C68">
     <sortCondition ref="A2"/>

</xml_diff>

<commit_message>
Complete test for table_variability macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="232">
   <si>
     <t>Test</t>
   </si>
@@ -126,12 +126,6 @@
     <t>Test stats table</t>
   </si>
   <si>
-    <t>Table_variability</t>
-  </si>
-  <si>
-    <t>Test variability table</t>
-  </si>
-  <si>
     <t>table_variability_test1</t>
   </si>
   <si>
@@ -706,6 +700,21 @@
   </si>
   <si>
     <t>Test Mean Absolute Deviation</t>
+  </si>
+  <si>
+    <t>Table_variability1</t>
+  </si>
+  <si>
+    <t>Test variability table for scale=252, digits=4</t>
+  </si>
+  <si>
+    <t>Table_variability2</t>
+  </si>
+  <si>
+    <t>table_variability_test2</t>
+  </si>
+  <si>
+    <t>Test variability table for scale=1, digits=8</t>
   </si>
 </sst>
 </file>
@@ -1030,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,156 +1065,156 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
         <v>85</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" t="s">
         <v>182</v>
-      </c>
-      <c r="C10" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
         <v>183</v>
-      </c>
-      <c r="C11" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" t="s">
         <v>149</v>
-      </c>
-      <c r="C14" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1216,12 +1225,12 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -1232,68 +1241,68 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
         <v>54</v>
-      </c>
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" t="s">
         <v>140</v>
-      </c>
-      <c r="B20" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" t="s">
         <v>162</v>
-      </c>
-      <c r="B22" t="s">
-        <v>163</v>
-      </c>
-      <c r="C22" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" t="s">
         <v>165</v>
-      </c>
-      <c r="B23" t="s">
-        <v>166</v>
-      </c>
-      <c r="C23" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1320,57 +1329,57 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
         <v>60</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
         <v>65</v>
-      </c>
-      <c r="B29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" t="s">
         <v>175</v>
-      </c>
-      <c r="B30" t="s">
-        <v>176</v>
-      </c>
-      <c r="C30" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1378,7 +1387,7 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
@@ -1389,7 +1398,7 @@
         <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
         <v>19</v>
@@ -1397,24 +1406,24 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" t="s">
         <v>115</v>
-      </c>
-      <c r="C33" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" t="s">
         <v>116</v>
-      </c>
-      <c r="C34" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1441,65 +1450,65 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" t="s">
         <v>74</v>
-      </c>
-      <c r="B40" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C42" t="s">
         <v>24</v>
@@ -1507,10 +1516,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
         <v>25</v>
@@ -1518,35 +1527,35 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" t="s">
         <v>168</v>
       </c>
-      <c r="B46" t="s">
-        <v>170</v>
-      </c>
       <c r="C46" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1554,7 +1563,7 @@
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C47" t="s">
         <v>21</v>
@@ -1565,7 +1574,7 @@
         <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C48" t="s">
         <v>23</v>
@@ -1573,263 +1582,263 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B49" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C49" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" t="s">
         <v>152</v>
       </c>
-      <c r="B50" t="s">
-        <v>154</v>
-      </c>
       <c r="C50" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C51" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B53" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>154</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
       <c r="C54" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B55" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>159</v>
+        <v>76</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="C56" t="s">
-        <v>161</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="B57" t="s">
         <v>133</v>
       </c>
       <c r="C57" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>135</v>
+        <v>49</v>
       </c>
       <c r="C58" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>186</v>
       </c>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="C59" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>187</v>
+      </c>
+      <c r="B60" t="s">
         <v>188</v>
       </c>
-      <c r="B60" t="s">
-        <v>187</v>
-      </c>
       <c r="C60" t="s">
-        <v>57</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B61" t="s">
+        <v>192</v>
+      </c>
+      <c r="C61" t="s">
         <v>190</v>
-      </c>
-      <c r="C61" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B63" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="C63" t="s">
-        <v>193</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B64" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C64" t="s">
-        <v>26</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B65" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B66" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C66" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B67" t="s">
+        <v>32</v>
+      </c>
+      <c r="C67" t="s">
         <v>208</v>
-      </c>
-      <c r="C67" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>209</v>
+        <v>81</v>
       </c>
       <c r="B68" t="s">
-        <v>32</v>
+        <v>210</v>
       </c>
       <c r="C68" t="s">
-        <v>210</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>209</v>
       </c>
       <c r="B69" t="s">
+        <v>211</v>
+      </c>
+      <c r="C69" t="s">
         <v>212</v>
-      </c>
-      <c r="C69" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B70" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C70" t="s">
-        <v>214</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" t="s">
         <v>215</v>
-      </c>
-      <c r="B71" t="s">
-        <v>216</v>
-      </c>
-      <c r="C71" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>33</v>
+        <v>216</v>
       </c>
       <c r="B72" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C72" t="s">
         <v>217</v>
@@ -1840,43 +1849,43 @@
         <v>218</v>
       </c>
       <c r="B73" t="s">
-        <v>31</v>
+        <v>219</v>
       </c>
       <c r="C73" t="s">
-        <v>219</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>221</v>
+      </c>
+      <c r="B74" t="s">
         <v>220</v>
       </c>
-      <c r="B74" t="s">
-        <v>221</v>
-      </c>
       <c r="C74" t="s">
-        <v>44</v>
+        <v>222</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>37</v>
+      </c>
+      <c r="B75" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" t="s">
         <v>223</v>
-      </c>
-      <c r="B75" t="s">
-        <v>222</v>
-      </c>
-      <c r="C75" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>39</v>
+        <v>225</v>
       </c>
       <c r="B76" t="s">
-        <v>40</v>
+        <v>226</v>
       </c>
       <c r="C76" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1887,7 +1896,18 @@
         <v>228</v>
       </c>
       <c r="C77" t="s">
-        <v>226</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>229</v>
+      </c>
+      <c r="B78" t="s">
+        <v>231</v>
+      </c>
+      <c r="C78" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add parameter digits to table_SpecificRisk macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -141,9 +141,6 @@
     <t>table_InformationRatio_test1</t>
   </si>
   <si>
-    <t>Table_SpecificRisk</t>
-  </si>
-  <si>
     <t>table_SpecificRisk_test1</t>
   </si>
   <si>
@@ -715,6 +712,9 @@
   </si>
   <si>
     <t>Test variability table for scale=1, digits=8</t>
+  </si>
+  <si>
+    <t>Table_SpecificRisk1</t>
   </si>
 </sst>
 </file>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,156 +1065,156 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
         <v>83</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>84</v>
-      </c>
-      <c r="C3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
         <v>90</v>
-      </c>
-      <c r="B4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" t="s">
         <v>92</v>
-      </c>
-      <c r="B5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" t="s">
         <v>122</v>
-      </c>
-      <c r="B8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C8" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
         <v>142</v>
       </c>
-      <c r="B12" t="s">
-        <v>143</v>
-      </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" t="s">
         <v>144</v>
       </c>
-      <c r="B13" t="s">
-        <v>145</v>
-      </c>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" t="s">
         <v>146</v>
       </c>
-      <c r="B14" t="s">
-        <v>147</v>
-      </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
         <v>106</v>
-      </c>
-      <c r="B15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1225,12 +1225,12 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -1241,68 +1241,68 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
         <v>52</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" t="s">
         <v>136</v>
       </c>
-      <c r="B19" t="s">
-        <v>137</v>
-      </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" t="s">
         <v>138</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>139</v>
-      </c>
-      <c r="C20" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" t="s">
         <v>171</v>
       </c>
-      <c r="B21" t="s">
-        <v>172</v>
-      </c>
       <c r="C21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" t="s">
         <v>160</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>161</v>
-      </c>
-      <c r="C22" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" t="s">
         <v>163</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>164</v>
-      </c>
-      <c r="C23" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1329,57 +1329,57 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
         <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
         <v>58</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>59</v>
-      </c>
-      <c r="C27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" t="s">
         <v>61</v>
-      </c>
-      <c r="B28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
         <v>63</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>64</v>
-      </c>
-      <c r="C29" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" t="s">
         <v>173</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>174</v>
-      </c>
-      <c r="C30" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1387,7 +1387,7 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
@@ -1398,7 +1398,7 @@
         <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C32" t="s">
         <v>19</v>
@@ -1406,24 +1406,24 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1450,65 +1450,65 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" t="s">
         <v>67</v>
-      </c>
-      <c r="B38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" t="s">
         <v>69</v>
-      </c>
-      <c r="B39" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" t="s">
         <v>94</v>
-      </c>
-      <c r="B41" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
         <v>24</v>
@@ -1516,10 +1516,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
         <v>25</v>
@@ -1527,35 +1527,35 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" t="s">
         <v>98</v>
-      </c>
-      <c r="B44" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" t="s">
         <v>100</v>
-      </c>
-      <c r="B45" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B46" t="s">
+        <v>167</v>
+      </c>
+      <c r="C46" t="s">
         <v>168</v>
-      </c>
-      <c r="C46" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1563,7 +1563,7 @@
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C47" t="s">
         <v>21</v>
@@ -1574,7 +1574,7 @@
         <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C48" t="s">
         <v>23</v>
@@ -1582,32 +1582,32 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B50" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" t="s">
         <v>152</v>
-      </c>
-      <c r="C50" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" t="s">
         <v>128</v>
-      </c>
-      <c r="B51" t="s">
-        <v>129</v>
       </c>
       <c r="C51" t="s">
         <v>36</v>
@@ -1615,79 +1615,79 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" t="s">
         <v>88</v>
-      </c>
-      <c r="B52" t="s">
-        <v>130</v>
-      </c>
-      <c r="C52" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C53" t="s">
-        <v>41</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B54" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C54" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>157</v>
+        <v>75</v>
       </c>
       <c r="B55" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="C55" t="s">
-        <v>159</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C56" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>132</v>
+        <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="C57" t="s">
-        <v>134</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>185</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>184</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1695,18 +1695,18 @@
         <v>186</v>
       </c>
       <c r="B59" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C59" t="s">
-        <v>55</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B60" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C60" t="s">
         <v>189</v>
@@ -1728,10 +1728,10 @@
         <v>195</v>
       </c>
       <c r="B62" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="C62" t="s">
-        <v>191</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1742,7 +1742,7 @@
         <v>203</v>
       </c>
       <c r="C63" t="s">
-        <v>26</v>
+        <v>199</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1769,98 +1769,98 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="B66" t="s">
-        <v>206</v>
+        <v>32</v>
       </c>
       <c r="C66" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>207</v>
+        <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>32</v>
+        <v>209</v>
       </c>
       <c r="C67" t="s">
-        <v>208</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>81</v>
+        <v>208</v>
       </c>
       <c r="B68" t="s">
         <v>210</v>
       </c>
       <c r="C68" t="s">
-        <v>82</v>
+        <v>211</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C69" t="s">
-        <v>212</v>
+        <v>39</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>213</v>
+        <v>33</v>
       </c>
       <c r="B70" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" t="s">
         <v>214</v>
-      </c>
-      <c r="C70" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>33</v>
+        <v>215</v>
       </c>
       <c r="B71" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C71" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B72" t="s">
-        <v>31</v>
+        <v>218</v>
       </c>
       <c r="C72" t="s">
-        <v>217</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B73" t="s">
         <v>219</v>
       </c>
       <c r="C73" t="s">
-        <v>42</v>
+        <v>221</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>221</v>
+        <v>37</v>
       </c>
       <c r="B74" t="s">
-        <v>220</v>
+        <v>38</v>
       </c>
       <c r="C74" t="s">
         <v>222</v>
@@ -1868,10 +1868,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>37</v>
+        <v>224</v>
       </c>
       <c r="B75" t="s">
-        <v>38</v>
+        <v>225</v>
       </c>
       <c r="C75" t="s">
         <v>223</v>
@@ -1879,35 +1879,35 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B76" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C76" t="s">
-        <v>224</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B77" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C77" t="s">
-        <v>35</v>
+        <v>229</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B78" t="s">
-        <v>231</v>
+        <v>166</v>
       </c>
       <c r="C78" t="s">
-        <v>230</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for max_drawdown macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="238">
   <si>
     <t>Test</t>
   </si>
@@ -715,6 +715,24 @@
   </si>
   <si>
     <t>Specific_Risk_test1</t>
+  </si>
+  <si>
+    <t>max_drawdown_test1</t>
+  </si>
+  <si>
+    <t>max_drawdown1</t>
+  </si>
+  <si>
+    <t>Test worst drawdown for simple returns</t>
+  </si>
+  <si>
+    <t>max_drawdown2</t>
+  </si>
+  <si>
+    <t>max_drawdown_test2</t>
+  </si>
+  <si>
+    <t>Test worst drawdown for compound returns</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1049,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1039,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1910,6 +1928,28 @@
         <v>129</v>
       </c>
     </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>233</v>
+      </c>
+      <c r="B79" t="s">
+        <v>234</v>
+      </c>
+      <c r="C79" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>235</v>
+      </c>
+      <c r="B80" t="s">
+        <v>237</v>
+      </c>
+      <c r="C80" t="s">
+        <v>236</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C78">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Complete test for Calmar_Ratio macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="244">
   <si>
     <t>Test</t>
   </si>
@@ -733,6 +733,24 @@
   </si>
   <si>
     <t>Test worst drawdown for compound returns</t>
+  </si>
+  <si>
+    <t>Calmar_Ratio_test1</t>
+  </si>
+  <si>
+    <t>Calmar Ratio1</t>
+  </si>
+  <si>
+    <t>Test Calmar ratio with scale=1</t>
+  </si>
+  <si>
+    <t>Calmar Ratio2</t>
+  </si>
+  <si>
+    <t>Test Calmar ratio with scale=252</t>
+  </si>
+  <si>
+    <t>Calmar_Ratio_test2</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1067,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1057,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1950,6 +1968,28 @@
         <v>236</v>
       </c>
     </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>239</v>
+      </c>
+      <c r="B81" t="s">
+        <v>240</v>
+      </c>
+      <c r="C81" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>241</v>
+      </c>
+      <c r="B82" t="s">
+        <v>242</v>
+      </c>
+      <c r="C82" t="s">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C78">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Complete test for Sterling_Ratio macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="250">
   <si>
     <t>Test</t>
   </si>
@@ -751,6 +751,24 @@
   </si>
   <si>
     <t>Calmar_Ratio_test2</t>
+  </si>
+  <si>
+    <t>Sterling Ratio1</t>
+  </si>
+  <si>
+    <t>Test Sterling ratio with scale=4</t>
+  </si>
+  <si>
+    <t>Sterling_Ratio_test1</t>
+  </si>
+  <si>
+    <t>Sterling Ratio2</t>
+  </si>
+  <si>
+    <t>Test Sterling ratio with scale=12</t>
+  </si>
+  <si>
+    <t>Sterling_Ratio_test2</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1085,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1075,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+      <selection activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1990,6 +2008,28 @@
         <v>243</v>
       </c>
     </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>244</v>
+      </c>
+      <c r="B83" t="s">
+        <v>245</v>
+      </c>
+      <c r="C83" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>247</v>
+      </c>
+      <c r="B84" t="s">
+        <v>248</v>
+      </c>
+      <c r="C84" t="s">
+        <v>249</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C78">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Complete test for Drawdown_Peak macro
Problem in R script - DrawdownPeak.R can only pass for one column data.
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="253">
   <si>
     <t>Test</t>
   </si>
@@ -769,6 +769,15 @@
   </si>
   <si>
     <t>Sterling_Ratio_test2</t>
+  </si>
+  <si>
+    <t>Drawdown_Peak_test1</t>
+  </si>
+  <si>
+    <t>Drawdown Peak1</t>
+  </si>
+  <si>
+    <t>Test drawdown_peak</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1094,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1093,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J83" sqref="J83"/>
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2030,6 +2039,17 @@
         <v>249</v>
       </c>
     </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>251</v>
+      </c>
+      <c r="B85" t="s">
+        <v>252</v>
+      </c>
+      <c r="C85" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C78">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Complete test for Pain_Index macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="256">
   <si>
     <t>Test</t>
   </si>
@@ -778,6 +778,15 @@
   </si>
   <si>
     <t>Test drawdown_peak</t>
+  </si>
+  <si>
+    <t>Pain_Index_test</t>
+  </si>
+  <si>
+    <t>Test pain index</t>
+  </si>
+  <si>
+    <t>Pain index</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1103,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1102,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2050,6 +2059,17 @@
         <v>250</v>
       </c>
     </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>255</v>
+      </c>
+      <c r="B86" t="s">
+        <v>254</v>
+      </c>
+      <c r="C86" t="s">
+        <v>253</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C78">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Complete test for Ulcer_Index macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="259">
   <si>
     <t>Test</t>
   </si>
@@ -787,6 +787,15 @@
   </si>
   <si>
     <t>Pain index</t>
+  </si>
+  <si>
+    <t>Ulcer index</t>
+  </si>
+  <si>
+    <t>Test ulcer index</t>
+  </si>
+  <si>
+    <t>Ulcer_Index_test</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1112,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1111,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2070,6 +2079,17 @@
         <v>253</v>
       </c>
     </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>256</v>
+      </c>
+      <c r="B87" t="s">
+        <v>257</v>
+      </c>
+      <c r="C87" t="s">
+        <v>258</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C78">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Complete test for Find_Drawdowns macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="265">
   <si>
     <t>Test</t>
   </si>
@@ -796,6 +796,24 @@
   </si>
   <si>
     <t>Ulcer_Index_test</t>
+  </si>
+  <si>
+    <t>Find_Drawdowns_test1</t>
+  </si>
+  <si>
+    <t>Test find drawdown for simple returns</t>
+  </si>
+  <si>
+    <t>Find_Drawdowns1</t>
+  </si>
+  <si>
+    <t>Find_Drawdowns2</t>
+  </si>
+  <si>
+    <t>Test find drawdown for compound returns</t>
+  </si>
+  <si>
+    <t>Find_Drawdowns_test2</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1130,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1120,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2090,6 +2108,28 @@
         <v>258</v>
       </c>
     </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>261</v>
+      </c>
+      <c r="B88" t="s">
+        <v>260</v>
+      </c>
+      <c r="C88" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>262</v>
+      </c>
+      <c r="B89" t="s">
+        <v>263</v>
+      </c>
+      <c r="C89" t="s">
+        <v>264</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C78">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Complete test for Sort_Drawdowns macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="268">
   <si>
     <t>Test</t>
   </si>
@@ -814,6 +814,15 @@
   </si>
   <si>
     <t>Find_Drawdowns_test2</t>
+  </si>
+  <si>
+    <t>Sort_Drawdowns</t>
+  </si>
+  <si>
+    <t>Test sort drawdown for simple returns</t>
+  </si>
+  <si>
+    <t>Sort_Drawdowns_test</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1139,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1138,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2130,6 +2139,17 @@
         <v>264</v>
       </c>
     </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>265</v>
+      </c>
+      <c r="B90" t="s">
+        <v>266</v>
+      </c>
+      <c r="C90" t="s">
+        <v>267</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C78">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Complete test for Table_Drawdowns macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="271">
   <si>
     <t>Test</t>
   </si>
@@ -823,6 +823,15 @@
   </si>
   <si>
     <t>Sort_Drawdowns_test</t>
+  </si>
+  <si>
+    <t>Table_Drawdowns_test</t>
+  </si>
+  <si>
+    <t>Test drawdown table</t>
+  </si>
+  <si>
+    <t>Table_Drawdowns</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1148,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1147,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2150,6 +2159,17 @@
         <v>267</v>
       </c>
     </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>270</v>
+      </c>
+      <c r="B91" t="s">
+        <v>269</v>
+      </c>
+      <c r="C91" t="s">
+        <v>268</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C78">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Change Drawdown_Peak to Drawdowns
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -771,15 +771,6 @@
     <t>Sterling_Ratio_test2</t>
   </si>
   <si>
-    <t>Drawdown_Peak_test1</t>
-  </si>
-  <si>
-    <t>Drawdown Peak1</t>
-  </si>
-  <si>
-    <t>Test drawdown_peak</t>
-  </si>
-  <si>
     <t>Pain_Index_test</t>
   </si>
   <si>
@@ -832,6 +823,15 @@
   </si>
   <si>
     <t>Table_Drawdowns</t>
+  </si>
+  <si>
+    <t>Drawdowns1</t>
+  </si>
+  <si>
+    <t>Test drawdowns</t>
+  </si>
+  <si>
+    <t>Drawdowns_test1</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1148,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1159,7 +1159,7 @@
   <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2095,79 +2095,79 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="B85" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="C85" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B86" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C86" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B87" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C87" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B88" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C88" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B89" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C89" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B90" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C90" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B91" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C91" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete test for Average_Drawdown macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="274">
   <si>
     <t>Test</t>
   </si>
@@ -832,6 +832,15 @@
   </si>
   <si>
     <t>Drawdowns_test1</t>
+  </si>
+  <si>
+    <t>Average_Drawdown_test</t>
+  </si>
+  <si>
+    <t>Test average drawdown</t>
+  </si>
+  <si>
+    <t>Average Drawdown</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1157,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1156,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2170,6 +2179,17 @@
         <v>265</v>
       </c>
     </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>273</v>
+      </c>
+      <c r="B92" t="s">
+        <v>272</v>
+      </c>
+      <c r="C92" t="s">
+        <v>271</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C78">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Create Drawdown_Deviation macro and add test
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="277">
   <si>
     <t>Test</t>
   </si>
@@ -841,6 +841,15 @@
   </si>
   <si>
     <t>Average Drawdown</t>
+  </si>
+  <si>
+    <t>Drawdown_Deviation_test</t>
+  </si>
+  <si>
+    <t>Test drawdown deviation</t>
+  </si>
+  <si>
+    <t>Drawdown Deviation</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1166,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1165,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2190,6 +2199,17 @@
         <v>271</v>
       </c>
     </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>276</v>
+      </c>
+      <c r="B93" t="s">
+        <v>275</v>
+      </c>
+      <c r="C93" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C78">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Average_length and Average_recovery created and tested
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rma\Desktop\SASPerformanceAnalytics\Performance Analytics Library\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19716" windowHeight="8004"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="283">
   <si>
     <t>Test</t>
   </si>
@@ -850,6 +855,24 @@
   </si>
   <si>
     <t>Drawdown Deviation</t>
+  </si>
+  <si>
+    <t>Average Length</t>
+  </si>
+  <si>
+    <t>Test average length</t>
+  </si>
+  <si>
+    <t>Average_Length_test</t>
+  </si>
+  <si>
+    <t>Average Recovery</t>
+  </si>
+  <si>
+    <t>Test average recovery</t>
+  </si>
+  <si>
+    <t>Average_Recovery_test</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1189,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1174,20 +1197,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>106</v>
       </c>
@@ -1209,7 +1232,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -1220,7 +1243,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1231,7 +1254,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -1242,7 +1265,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>226</v>
       </c>
@@ -1253,7 +1276,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>169</v>
       </c>
@@ -1264,7 +1287,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>170</v>
       </c>
@@ -1275,7 +1298,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>171</v>
       </c>
@@ -1286,7 +1309,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>137</v>
       </c>
@@ -1297,7 +1320,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -1308,7 +1331,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -1319,7 +1342,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -1330,7 +1353,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1341,7 +1364,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>177</v>
       </c>
@@ -1352,7 +1375,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -1363,7 +1386,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -1374,7 +1397,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>133</v>
       </c>
@@ -1385,7 +1408,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>229</v>
       </c>
@@ -1396,7 +1419,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>164</v>
       </c>
@@ -1407,7 +1430,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -1418,7 +1441,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>158</v>
       </c>
@@ -1429,7 +1452,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>218</v>
       </c>
@@ -1440,7 +1463,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>179</v>
       </c>
@@ -1451,7 +1474,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>180</v>
       </c>
@@ -1462,7 +1485,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>187</v>
       </c>
@@ -1473,7 +1496,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>188</v>
       </c>
@@ -1484,7 +1507,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1495,7 +1518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1506,7 +1529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1517,7 +1540,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -1528,7 +1551,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -1539,7 +1562,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -1550,7 +1573,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>166</v>
       </c>
@@ -1561,7 +1584,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1572,7 +1595,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -1583,7 +1606,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -1594,7 +1617,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -1605,7 +1628,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -1616,7 +1639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -1627,7 +1650,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -1638,7 +1661,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>64</v>
       </c>
@@ -1649,7 +1672,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -1660,7 +1683,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -1671,7 +1694,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -1682,7 +1705,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -1693,7 +1716,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -1704,7 +1727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -1715,7 +1738,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -1726,7 +1749,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>230</v>
       </c>
@@ -1737,7 +1760,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -1748,7 +1771,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -1759,7 +1782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>227</v>
       </c>
@@ -1770,7 +1793,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>228</v>
       </c>
@@ -1781,7 +1804,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -1792,7 +1815,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>145</v>
       </c>
@@ -1803,7 +1826,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>189</v>
       </c>
@@ -1814,7 +1837,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>190</v>
       </c>
@@ -1825,7 +1848,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>191</v>
       </c>
@@ -1836,7 +1859,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>192</v>
       </c>
@@ -1847,7 +1870,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>200</v>
       </c>
@@ -1858,7 +1881,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>211</v>
       </c>
@@ -1869,7 +1892,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>214</v>
       </c>
@@ -1880,7 +1903,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>78</v>
       </c>
@@ -1891,7 +1914,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>202</v>
       </c>
@@ -1902,7 +1925,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>209</v>
       </c>
@@ -1913,7 +1936,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>123</v>
       </c>
@@ -1924,7 +1947,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -1935,7 +1958,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>37</v>
       </c>
@@ -1946,7 +1969,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>206</v>
       </c>
@@ -1957,7 +1980,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>225</v>
       </c>
@@ -1968,7 +1991,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>33</v>
       </c>
@@ -1979,7 +2002,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>220</v>
       </c>
@@ -1990,7 +2013,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>222</v>
       </c>
@@ -2001,7 +2024,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>149</v>
       </c>
@@ -2012,7 +2035,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>152</v>
       </c>
@@ -2023,7 +2046,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -2034,7 +2057,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>127</v>
       </c>
@@ -2045,7 +2068,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>233</v>
       </c>
@@ -2056,7 +2079,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>235</v>
       </c>
@@ -2067,7 +2090,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>239</v>
       </c>
@@ -2078,7 +2101,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>241</v>
       </c>
@@ -2089,7 +2112,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>244</v>
       </c>
@@ -2100,7 +2123,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>247</v>
       </c>
@@ -2111,7 +2134,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>268</v>
       </c>
@@ -2122,7 +2145,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>252</v>
       </c>
@@ -2133,7 +2156,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>253</v>
       </c>
@@ -2144,7 +2167,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>258</v>
       </c>
@@ -2155,7 +2178,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>259</v>
       </c>
@@ -2166,7 +2189,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>262</v>
       </c>
@@ -2177,7 +2200,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>267</v>
       </c>
@@ -2188,7 +2211,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>273</v>
       </c>
@@ -2199,7 +2222,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>276</v>
       </c>
@@ -2208,6 +2231,28 @@
       </c>
       <c r="C93" t="s">
         <v>274</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>277</v>
+      </c>
+      <c r="B94" t="s">
+        <v>278</v>
+      </c>
+      <c r="C94" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>280</v>
+      </c>
+      <c r="B95" t="s">
+        <v>281</v>
+      </c>
+      <c r="C95" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add NET parameter for MSquared macro and create tests
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -543,18 +543,12 @@
     <t>CAPM_epsilon1</t>
   </si>
   <si>
-    <t>Test Msquared with method=discrete, scale=252</t>
-  </si>
-  <si>
     <t>Msquared1</t>
   </si>
   <si>
     <t>Msquared2</t>
   </si>
   <si>
-    <t>Test Msquared with method=discrete, scale=1</t>
-  </si>
-  <si>
     <t>Msquared_test2</t>
   </si>
   <si>
@@ -564,12 +558,6 @@
     <t>Msquared_test4</t>
   </si>
   <si>
-    <t>Test Msquared with method=log, scale=4</t>
-  </si>
-  <si>
-    <t>Test Msquared with method=log, scale=12</t>
-  </si>
-  <si>
     <t>Msquared3</t>
   </si>
   <si>
@@ -868,6 +856,18 @@
   </si>
   <si>
     <t>Test distributions table</t>
+  </si>
+  <si>
+    <t>Test Msquared with method=log, scale=12,NET=FALSE</t>
+  </si>
+  <si>
+    <t>Test Msquared with method=log, scale=4,NET=TRUE</t>
+  </si>
+  <si>
+    <t>Test Msquared with method=discrete, scale=252, NET=TRUE</t>
+  </si>
+  <si>
+    <t>Test Msquared with method=discrete, scale=1,NET=FALSE</t>
   </si>
 </sst>
 </file>
@@ -1184,7 +1184,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1194,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1262,10 +1262,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -1273,24 +1273,24 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B7" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C7" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B8" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C8" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1328,13 +1328,13 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B12" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C12" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1383,24 +1383,24 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B17" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C17" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B18" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C18" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1460,57 +1460,57 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B24" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C24" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C25" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B26" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C26" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B27" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C27" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B28" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C28" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1548,43 +1548,43 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B32" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C32" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B33" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C33" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B34" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C34" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>281</v>
       </c>
       <c r="C35" t="s">
         <v>49</v>
@@ -1592,46 +1592,46 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" t="s">
+        <v>282</v>
+      </c>
+      <c r="C36" t="s">
         <v>176</v>
-      </c>
-      <c r="B36" t="s">
-        <v>177</v>
-      </c>
-      <c r="C36" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B37" t="s">
-        <v>181</v>
+        <v>280</v>
       </c>
       <c r="C37" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B38" t="s">
-        <v>182</v>
+        <v>279</v>
       </c>
       <c r="C38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B39" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C39" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1878,24 +1878,24 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B62" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C62" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B63" t="s">
         <v>158</v>
       </c>
       <c r="C63" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1922,7 +1922,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B66" t="s">
         <v>118</v>
@@ -1933,7 +1933,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B67" t="s">
         <v>119</v>
@@ -1944,24 +1944,24 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B68" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C68" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B69" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C69" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1988,10 +1988,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B72" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C72" t="s">
         <v>26</v>
@@ -1999,54 +1999,54 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B73" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C73" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B74" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C74" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B75" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C75" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B76" t="s">
         <v>32</v>
       </c>
       <c r="C76" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B77" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C77" t="s">
         <v>41</v>
@@ -2054,13 +2054,13 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B78" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C78" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -2068,7 +2068,7 @@
         <v>75</v>
       </c>
       <c r="B79" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C79" t="s">
         <v>76</v>
@@ -2076,24 +2076,24 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B80" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C80" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B81" t="s">
         <v>31</v>
       </c>
       <c r="C81" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -2101,7 +2101,7 @@
         <v>120</v>
       </c>
       <c r="B82" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C82" t="s">
         <v>36</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B84" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C84" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -2137,15 +2137,15 @@
         <v>38</v>
       </c>
       <c r="C85" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B86" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C86" t="s">
         <v>39</v>
@@ -2153,7 +2153,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B87" t="s">
         <v>157</v>
@@ -2170,15 +2170,15 @@
         <v>34</v>
       </c>
       <c r="C88" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B89" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C89" t="s">
         <v>35</v>
@@ -2186,13 +2186,13 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B90" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C90" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -2241,13 +2241,13 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B95" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C95" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add tests to CAPM_JensenAlpha for monthly and yearly returns
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="289">
   <si>
     <t>Test</t>
   </si>
@@ -159,12 +159,6 @@
     <t>appraisal_ratio_test1</t>
   </si>
   <si>
-    <t>CAPM_JensenAlpha</t>
-  </si>
-  <si>
-    <t>Test Jensen Alpha</t>
-  </si>
-  <si>
     <t>CAPM_JensenAlpha_test1</t>
   </si>
   <si>
@@ -525,15 +519,6 @@
     <t>appraisal ratio3</t>
   </si>
   <si>
-    <t>Test appraisal ratio with option=appraisal</t>
-  </si>
-  <si>
-    <t>Test appraisal ratio with option=modified</t>
-  </si>
-  <si>
-    <t>Test appraisal ratio with option=alternative</t>
-  </si>
-  <si>
     <t>appraisal_ratio_test2</t>
   </si>
   <si>
@@ -868,6 +853,39 @@
   </si>
   <si>
     <t>Test Msquared with method=discrete, scale=1,NET=FALSE</t>
+  </si>
+  <si>
+    <t>Test appraisal ratio for daily returnswith option=appraisal</t>
+  </si>
+  <si>
+    <t>Test appraisal ratio for monthly returns with option=modified</t>
+  </si>
+  <si>
+    <t>Test appraisal ratio for yearly returns with option=alternative</t>
+  </si>
+  <si>
+    <t>CAPM_JensenAlpha1</t>
+  </si>
+  <si>
+    <t>Test Jensen Alpha for daily returns</t>
+  </si>
+  <si>
+    <t>CAPM_JensenAlpha2</t>
+  </si>
+  <si>
+    <t>CAPM_JensenAlpha3</t>
+  </si>
+  <si>
+    <t>Test Jensen Alpha for monthly returns</t>
+  </si>
+  <si>
+    <t>Test Jensen Alpha for yearly returns</t>
+  </si>
+  <si>
+    <t>CAPM_JensenAlpha_test2</t>
+  </si>
+  <si>
+    <t>CAPM_JensenAlpha_test3</t>
   </si>
 </sst>
 </file>
@@ -1192,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1218,7 +1236,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
@@ -1229,43 +1247,43 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
         <v>77</v>
-      </c>
-      <c r="B3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -1273,32 +1291,32 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C7" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B8" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C8" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>278</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
@@ -1306,101 +1324,101 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" t="s">
+        <v>279</v>
+      </c>
+      <c r="C10" t="s">
         <v>166</v>
-      </c>
-      <c r="B10" t="s">
-        <v>169</v>
-      </c>
-      <c r="C10" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" t="s">
         <v>167</v>
-      </c>
-      <c r="B11" t="s">
-        <v>170</v>
-      </c>
-      <c r="C11" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B12" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C12" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" t="s">
         <v>138</v>
-      </c>
-      <c r="C15" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B17" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C17" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B18" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C18" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1411,12 +1429,12 @@
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -1427,13 +1445,13 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1444,59 +1462,59 @@
         <v>128</v>
       </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>262</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>261</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="B24" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="C24" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B25" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C25" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="B26" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="C26" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B27" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C27" t="s">
         <v>247</v>
@@ -1504,156 +1522,156 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>250</v>
+        <v>158</v>
       </c>
       <c r="B28" t="s">
-        <v>251</v>
+        <v>159</v>
       </c>
       <c r="C28" t="s">
-        <v>252</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C29" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C30" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>154</v>
+        <v>219</v>
       </c>
       <c r="B31" t="s">
-        <v>155</v>
+        <v>220</v>
       </c>
       <c r="C31" t="s">
-        <v>156</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B32" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="B33" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="C33" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>210</v>
+        <v>169</v>
       </c>
       <c r="B34" t="s">
-        <v>211</v>
+        <v>276</v>
       </c>
       <c r="C34" t="s">
-        <v>209</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B36" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C36" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B37" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C37" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>180</v>
+        <v>238</v>
       </c>
       <c r="B38" t="s">
-        <v>279</v>
+        <v>237</v>
       </c>
       <c r="C38" t="s">
-        <v>178</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>243</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>242</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>241</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1661,18 +1679,18 @@
         <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
         <v>54</v>
@@ -1683,109 +1701,109 @@
         <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="B45" t="s">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="C45" t="s">
-        <v>59</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>162</v>
+        <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>163</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>164</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>110</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C51" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>114</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1801,24 +1819,24 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
         <v>67</v>
       </c>
       <c r="C55" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C56" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1826,32 +1844,32 @@
         <v>88</v>
       </c>
       <c r="B57" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C58" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B59" t="s">
         <v>97</v>
       </c>
       <c r="C59" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1859,7 +1877,7 @@
         <v>92</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C60" t="s">
         <v>93</v>
@@ -1867,219 +1885,219 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>248</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
+        <v>249</v>
       </c>
       <c r="C61" t="s">
-        <v>95</v>
+        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="B62" t="s">
-        <v>254</v>
+        <v>156</v>
       </c>
       <c r="C62" t="s">
-        <v>255</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>221</v>
+        <v>20</v>
       </c>
       <c r="B63" t="s">
-        <v>158</v>
+        <v>114</v>
       </c>
       <c r="C63" t="s">
-        <v>222</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C64" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>22</v>
+        <v>214</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C65" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B66" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C66" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="B67" t="s">
-        <v>119</v>
+        <v>231</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>232</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>233</v>
+      </c>
+      <c r="B68" t="s">
+        <v>234</v>
+      </c>
+      <c r="C68" t="s">
         <v>235</v>
-      </c>
-      <c r="B68" t="s">
-        <v>236</v>
-      </c>
-      <c r="C68" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>238</v>
+        <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>239</v>
+        <v>140</v>
       </c>
       <c r="C69" t="s">
-        <v>240</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>139</v>
       </c>
       <c r="B70" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" t="s">
         <v>142</v>
-      </c>
-      <c r="C70" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="C71" t="s">
-        <v>144</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B72" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C72" t="s">
-        <v>26</v>
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B73" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C73" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B74" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C74" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B75" t="s">
-        <v>191</v>
+        <v>32</v>
       </c>
       <c r="C75" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B76" t="s">
-        <v>32</v>
+        <v>199</v>
       </c>
       <c r="C76" t="s">
-        <v>193</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B77" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C77" t="s">
-        <v>41</v>
+        <v>202</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>206</v>
+        <v>73</v>
       </c>
       <c r="B78" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C78" t="s">
-        <v>207</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>189</v>
       </c>
       <c r="B79" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C79" t="s">
-        <v>76</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B80" t="s">
-        <v>196</v>
+        <v>31</v>
       </c>
       <c r="C80" t="s">
         <v>197</v>
@@ -2087,167 +2105,189 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>201</v>
+        <v>118</v>
       </c>
       <c r="B81" t="s">
-        <v>31</v>
+        <v>273</v>
       </c>
       <c r="C81" t="s">
-        <v>202</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>278</v>
+        <v>119</v>
       </c>
       <c r="C82" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>253</v>
       </c>
       <c r="B83" t="s">
-        <v>121</v>
+        <v>252</v>
       </c>
       <c r="C83" t="s">
-        <v>83</v>
+        <v>251</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>258</v>
+        <v>37</v>
       </c>
       <c r="B84" t="s">
-        <v>257</v>
+        <v>38</v>
       </c>
       <c r="C84" t="s">
-        <v>256</v>
+        <v>203</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>37</v>
+        <v>193</v>
       </c>
       <c r="B85" t="s">
-        <v>38</v>
+        <v>194</v>
       </c>
       <c r="C85" t="s">
-        <v>208</v>
+        <v>39</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B86" t="s">
-        <v>199</v>
+        <v>155</v>
       </c>
       <c r="C86" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>217</v>
+        <v>33</v>
       </c>
       <c r="B87" t="s">
-        <v>157</v>
+        <v>34</v>
       </c>
       <c r="C87" t="s">
-        <v>40</v>
+        <v>195</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>33</v>
+        <v>207</v>
       </c>
       <c r="B88" t="s">
-        <v>34</v>
+        <v>208</v>
       </c>
       <c r="C88" t="s">
-        <v>200</v>
+        <v>35</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B89" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C89" t="s">
-        <v>35</v>
+        <v>210</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
       <c r="B90" t="s">
-        <v>216</v>
+        <v>144</v>
       </c>
       <c r="C90" t="s">
-        <v>215</v>
+        <v>145</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B91" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C91" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
       <c r="B92" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="C92" t="s">
-        <v>150</v>
+        <v>69</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>70</v>
+        <v>121</v>
       </c>
       <c r="B93" t="s">
         <v>122</v>
       </c>
       <c r="C93" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>123</v>
+        <v>239</v>
       </c>
       <c r="B94" t="s">
-        <v>124</v>
+        <v>240</v>
       </c>
       <c r="C94" t="s">
-        <v>125</v>
+        <v>241</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>244</v>
+        <v>281</v>
       </c>
       <c r="B95" t="s">
-        <v>245</v>
+        <v>282</v>
       </c>
       <c r="C95" t="s">
-        <v>246</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>283</v>
+      </c>
+      <c r="B96" t="s">
+        <v>285</v>
+      </c>
+      <c r="C96" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>284</v>
+      </c>
+      <c r="B97" t="s">
+        <v>286</v>
+      </c>
+      <c r="C97" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit for table_SpecificRisk macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -486,9 +486,6 @@
     <t>Information_Ratio_test2</t>
   </si>
   <si>
-    <t>Test Specific Risk table with scale=252</t>
-  </si>
-  <si>
     <t>Test Specific Risk with scale=252</t>
   </si>
   <si>
@@ -886,6 +883,9 @@
   </si>
   <si>
     <t>CAPM_JensenAlpha_test3</t>
+  </si>
+  <si>
+    <t>Test Specific Risk table for daily returns</t>
   </si>
 </sst>
 </file>
@@ -1212,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,10 +1280,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -1291,32 +1291,32 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B7" t="s">
         <v>267</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>268</v>
-      </c>
-      <c r="C7" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" t="s">
         <v>270</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>271</v>
-      </c>
-      <c r="C8" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
@@ -1324,35 +1324,35 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1401,24 +1401,24 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B17" t="s">
         <v>225</v>
       </c>
-      <c r="B17" t="s">
-        <v>226</v>
-      </c>
       <c r="C17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" t="s">
         <v>227</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>228</v>
-      </c>
-      <c r="C18" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1434,7 +1434,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -1467,68 +1467,68 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>253</v>
+      </c>
+      <c r="B24" t="s">
         <v>254</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>255</v>
-      </c>
-      <c r="C24" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>262</v>
+      </c>
+      <c r="B25" t="s">
         <v>263</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>264</v>
-      </c>
-      <c r="C25" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>244</v>
+      </c>
+      <c r="B27" t="s">
         <v>245</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>246</v>
-      </c>
-      <c r="C27" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>157</v>
+      </c>
+      <c r="B28" t="s">
         <v>158</v>
       </c>
-      <c r="B28" t="s">
-        <v>159</v>
-      </c>
       <c r="C28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1555,43 +1555,43 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>218</v>
+      </c>
+      <c r="B31" t="s">
         <v>219</v>
       </c>
-      <c r="B31" t="s">
-        <v>220</v>
-      </c>
       <c r="C31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>220</v>
+      </c>
+      <c r="B32" t="s">
+        <v>222</v>
+      </c>
+      <c r="C32" t="s">
         <v>221</v>
-      </c>
-      <c r="B32" t="s">
-        <v>223</v>
-      </c>
-      <c r="C32" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>204</v>
+      </c>
+      <c r="B33" t="s">
         <v>205</v>
       </c>
-      <c r="B33" t="s">
-        <v>206</v>
-      </c>
       <c r="C33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B34" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C34" t="s">
         <v>47</v>
@@ -1599,46 +1599,46 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" t="s">
+        <v>276</v>
+      </c>
+      <c r="C35" t="s">
         <v>170</v>
-      </c>
-      <c r="B35" t="s">
-        <v>277</v>
-      </c>
-      <c r="C35" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B36" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B37" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B38" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1709,13 +1709,13 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" t="s">
         <v>160</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>161</v>
-      </c>
-      <c r="C45" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1885,24 +1885,24 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>247</v>
+      </c>
+      <c r="B61" t="s">
         <v>248</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>249</v>
-      </c>
-      <c r="C61" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>215</v>
+      </c>
+      <c r="B62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" t="s">
         <v>216</v>
-      </c>
-      <c r="B62" t="s">
-        <v>156</v>
-      </c>
-      <c r="C62" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1929,7 +1929,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B65" t="s">
         <v>116</v>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B66" t="s">
         <v>117</v>
@@ -1951,24 +1951,24 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>229</v>
+      </c>
+      <c r="B67" t="s">
         <v>230</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>231</v>
-      </c>
-      <c r="C67" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>232</v>
+      </c>
+      <c r="B68" t="s">
         <v>233</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>234</v>
-      </c>
-      <c r="C68" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1995,10 +1995,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B71" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C71" t="s">
         <v>26</v>
@@ -2006,54 +2006,54 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B72" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C72" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B73" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C73" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B74" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C74" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B75" t="s">
         <v>32</v>
       </c>
       <c r="C75" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>197</v>
+      </c>
+      <c r="B76" t="s">
         <v>198</v>
-      </c>
-      <c r="B76" t="s">
-        <v>199</v>
       </c>
       <c r="C76" t="s">
         <v>41</v>
@@ -2061,13 +2061,13 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>200</v>
+      </c>
+      <c r="B77" t="s">
+        <v>199</v>
+      </c>
+      <c r="C77" t="s">
         <v>201</v>
-      </c>
-      <c r="B77" t="s">
-        <v>200</v>
-      </c>
-      <c r="C77" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -2075,7 +2075,7 @@
         <v>73</v>
       </c>
       <c r="B78" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C78" t="s">
         <v>74</v>
@@ -2083,24 +2083,24 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B79" t="s">
+        <v>190</v>
+      </c>
+      <c r="C79" t="s">
         <v>191</v>
-      </c>
-      <c r="C79" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B80" t="s">
         <v>31</v>
       </c>
       <c r="C80" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -2108,7 +2108,7 @@
         <v>118</v>
       </c>
       <c r="B81" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C81" t="s">
         <v>36</v>
@@ -2127,13 +2127,13 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B83" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C83" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -2144,15 +2144,15 @@
         <v>38</v>
       </c>
       <c r="C84" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>192</v>
+      </c>
+      <c r="B85" t="s">
         <v>193</v>
-      </c>
-      <c r="B85" t="s">
-        <v>194</v>
       </c>
       <c r="C85" t="s">
         <v>39</v>
@@ -2160,112 +2160,112 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>212</v>
+        <v>33</v>
       </c>
       <c r="B86" t="s">
-        <v>155</v>
+        <v>34</v>
       </c>
       <c r="C86" t="s">
-        <v>40</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>33</v>
+        <v>206</v>
       </c>
       <c r="B87" t="s">
-        <v>34</v>
+        <v>207</v>
       </c>
       <c r="C87" t="s">
-        <v>195</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B88" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C88" t="s">
-        <v>35</v>
+        <v>209</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>209</v>
+        <v>143</v>
       </c>
       <c r="B89" t="s">
-        <v>211</v>
+        <v>144</v>
       </c>
       <c r="C89" t="s">
-        <v>210</v>
+        <v>145</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B90" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C90" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>146</v>
+        <v>68</v>
       </c>
       <c r="B91" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="C91" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="B92" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C92" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>121</v>
+        <v>238</v>
       </c>
       <c r="B93" t="s">
-        <v>122</v>
+        <v>239</v>
       </c>
       <c r="C93" t="s">
-        <v>123</v>
+        <v>240</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>239</v>
+        <v>280</v>
       </c>
       <c r="B94" t="s">
-        <v>240</v>
+        <v>281</v>
       </c>
       <c r="C94" t="s">
-        <v>241</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B95" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C95" t="s">
-        <v>46</v>
+        <v>286</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -2281,13 +2281,13 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>284</v>
+        <v>211</v>
       </c>
       <c r="B97" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C97" t="s">
-        <v>288</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create D_Ratio macro and add test
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="310">
   <si>
     <t>Test</t>
   </si>
@@ -486,9 +486,6 @@
     <t>Information_Ratio_test2</t>
   </si>
   <si>
-    <t>Test Specific Risk with scale=252</t>
-  </si>
-  <si>
     <t>geo_mean_test</t>
   </si>
   <si>
@@ -886,6 +883,72 @@
   </si>
   <si>
     <t>Test Specific Risk table for daily returns</t>
+  </si>
+  <si>
+    <t>Test Specific Risk for daily returns</t>
+  </si>
+  <si>
+    <t>Test Specific Risk for monthly returns</t>
+  </si>
+  <si>
+    <t>Specific_Risk_test2</t>
+  </si>
+  <si>
+    <t>Specific_Risk2</t>
+  </si>
+  <si>
+    <t>Specific_Risk3</t>
+  </si>
+  <si>
+    <t>Test Specific Risk for yearly returns</t>
+  </si>
+  <si>
+    <t>Specific_Risk_test3</t>
+  </si>
+  <si>
+    <t>Total_Risk1</t>
+  </si>
+  <si>
+    <t>Test Total Risk with VARDEF=DF</t>
+  </si>
+  <si>
+    <t>Total_Risk_test1</t>
+  </si>
+  <si>
+    <t>Total_Risk2</t>
+  </si>
+  <si>
+    <t>Test Total Risk with VARDEF=N</t>
+  </si>
+  <si>
+    <t>Total_Risk_test2</t>
+  </si>
+  <si>
+    <t>Average_Length_test</t>
+  </si>
+  <si>
+    <t>Average Length</t>
+  </si>
+  <si>
+    <t>Test Average length</t>
+  </si>
+  <si>
+    <t>Average Recovery</t>
+  </si>
+  <si>
+    <t>Test Average Reconvery</t>
+  </si>
+  <si>
+    <t>Average_Recovery_test</t>
+  </si>
+  <si>
+    <t>D_Ratio_test</t>
+  </si>
+  <si>
+    <t>Test d ratio</t>
+  </si>
+  <si>
+    <t>D Ratio</t>
   </si>
 </sst>
 </file>
@@ -1210,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,10 +1343,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -1291,32 +1354,32 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B7" t="s">
         <v>266</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>267</v>
-      </c>
-      <c r="C7" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B8" t="s">
         <v>269</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>270</v>
-      </c>
-      <c r="C8" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
@@ -1324,35 +1387,35 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1401,24 +1464,24 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" t="s">
         <v>224</v>
       </c>
-      <c r="B17" t="s">
-        <v>225</v>
-      </c>
       <c r="C17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B18" t="s">
         <v>226</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>227</v>
-      </c>
-      <c r="C18" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1434,7 +1497,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -1467,68 +1530,68 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B24" t="s">
         <v>253</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>254</v>
-      </c>
-      <c r="C24" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>261</v>
+      </c>
+      <c r="B25" t="s">
         <v>262</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>263</v>
-      </c>
-      <c r="C25" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>243</v>
+      </c>
+      <c r="B27" t="s">
         <v>244</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>245</v>
-      </c>
-      <c r="C27" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" t="s">
         <v>157</v>
       </c>
-      <c r="B28" t="s">
-        <v>158</v>
-      </c>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1555,43 +1618,43 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>217</v>
+      </c>
+      <c r="B31" t="s">
         <v>218</v>
       </c>
-      <c r="B31" t="s">
-        <v>219</v>
-      </c>
       <c r="C31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>219</v>
+      </c>
+      <c r="B32" t="s">
+        <v>221</v>
+      </c>
+      <c r="C32" t="s">
         <v>220</v>
-      </c>
-      <c r="B32" t="s">
-        <v>222</v>
-      </c>
-      <c r="C32" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>203</v>
+      </c>
+      <c r="B33" t="s">
         <v>204</v>
       </c>
-      <c r="B33" t="s">
-        <v>205</v>
-      </c>
       <c r="C33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C34" t="s">
         <v>47</v>
@@ -1599,46 +1662,46 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" t="s">
+        <v>275</v>
+      </c>
+      <c r="C35" t="s">
         <v>169</v>
-      </c>
-      <c r="B35" t="s">
-        <v>276</v>
-      </c>
-      <c r="C35" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B36" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B37" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1709,13 +1772,13 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>158</v>
+      </c>
+      <c r="B45" t="s">
         <v>159</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>160</v>
-      </c>
-      <c r="C45" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1885,46 +1948,46 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>246</v>
+      </c>
+      <c r="B61" t="s">
         <v>247</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>248</v>
-      </c>
-      <c r="C61" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>215</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="C62" t="s">
-        <v>216</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B63" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C63" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>22</v>
+        <v>212</v>
       </c>
       <c r="B64" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1932,65 +1995,65 @@
         <v>213</v>
       </c>
       <c r="B65" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C65" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="B66" t="s">
-        <v>117</v>
+        <v>229</v>
       </c>
       <c r="C66" t="s">
-        <v>113</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B67" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C67" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>233</v>
+        <v>140</v>
       </c>
       <c r="C68" t="s">
-        <v>234</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>139</v>
       </c>
       <c r="B69" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C69" t="s">
-        <v>70</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="B70" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="C70" t="s">
-        <v>142</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -2001,7 +2064,7 @@
         <v>182</v>
       </c>
       <c r="C71" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -2028,233 +2091,233 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="B74" t="s">
-        <v>185</v>
+        <v>32</v>
       </c>
       <c r="C74" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B75" t="s">
-        <v>32</v>
+        <v>197</v>
       </c>
       <c r="C75" t="s">
-        <v>187</v>
+        <v>41</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B76" t="s">
         <v>198</v>
       </c>
       <c r="C76" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>200</v>
+        <v>73</v>
       </c>
       <c r="B77" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C77" t="s">
-        <v>201</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>187</v>
       </c>
       <c r="B78" t="s">
         <v>189</v>
       </c>
       <c r="C78" t="s">
-        <v>74</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B79" t="s">
-        <v>190</v>
+        <v>31</v>
       </c>
       <c r="C79" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>195</v>
+        <v>118</v>
       </c>
       <c r="B80" t="s">
-        <v>31</v>
+        <v>271</v>
       </c>
       <c r="C80" t="s">
-        <v>196</v>
+        <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>272</v>
+        <v>119</v>
       </c>
       <c r="C81" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>251</v>
       </c>
       <c r="B82" t="s">
-        <v>119</v>
+        <v>250</v>
       </c>
       <c r="C82" t="s">
-        <v>81</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>252</v>
+        <v>37</v>
       </c>
       <c r="B83" t="s">
-        <v>251</v>
+        <v>38</v>
       </c>
       <c r="C83" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>37</v>
+        <v>191</v>
       </c>
       <c r="B84" t="s">
-        <v>38</v>
+        <v>192</v>
       </c>
       <c r="C84" t="s">
-        <v>202</v>
+        <v>39</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>192</v>
+        <v>33</v>
       </c>
       <c r="B85" t="s">
+        <v>34</v>
+      </c>
+      <c r="C85" t="s">
         <v>193</v>
-      </c>
-      <c r="C85" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>33</v>
+        <v>205</v>
       </c>
       <c r="B86" t="s">
-        <v>34</v>
+        <v>206</v>
       </c>
       <c r="C86" t="s">
-        <v>194</v>
+        <v>35</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B87" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C87" t="s">
-        <v>35</v>
+        <v>208</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>208</v>
+        <v>143</v>
       </c>
       <c r="B88" t="s">
-        <v>210</v>
+        <v>144</v>
       </c>
       <c r="C88" t="s">
-        <v>209</v>
+        <v>145</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B89" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C89" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>146</v>
+        <v>68</v>
       </c>
       <c r="B90" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="C90" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="B91" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C91" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>121</v>
+        <v>237</v>
       </c>
       <c r="B92" t="s">
-        <v>122</v>
+        <v>238</v>
       </c>
       <c r="C92" t="s">
-        <v>123</v>
+        <v>239</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>238</v>
+        <v>279</v>
       </c>
       <c r="B93" t="s">
-        <v>239</v>
+        <v>280</v>
       </c>
       <c r="C93" t="s">
-        <v>240</v>
+        <v>46</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B94" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C94" t="s">
-        <v>46</v>
+        <v>285</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -2270,24 +2333,101 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>283</v>
+        <v>210</v>
       </c>
       <c r="B96" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C96" t="s">
-        <v>287</v>
+        <v>40</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B97" t="s">
         <v>288</v>
       </c>
       <c r="C97" t="s">
-        <v>40</v>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>291</v>
+      </c>
+      <c r="B98" t="s">
+        <v>289</v>
+      </c>
+      <c r="C98" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>292</v>
+      </c>
+      <c r="B99" t="s">
+        <v>293</v>
+      </c>
+      <c r="C99" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>295</v>
+      </c>
+      <c r="B100" t="s">
+        <v>296</v>
+      </c>
+      <c r="C100" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>298</v>
+      </c>
+      <c r="B101" t="s">
+        <v>299</v>
+      </c>
+      <c r="C101" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>302</v>
+      </c>
+      <c r="B102" t="s">
+        <v>303</v>
+      </c>
+      <c r="C102" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>304</v>
+      </c>
+      <c r="B103" t="s">
+        <v>305</v>
+      </c>
+      <c r="C103" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>309</v>
+      </c>
+      <c r="B104" t="s">
+        <v>308</v>
+      </c>
+      <c r="C104" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create BernadoLedoit_Ratio macro and add test
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="313">
   <si>
     <t>Test</t>
   </si>
@@ -949,6 +949,15 @@
   </si>
   <si>
     <t>D Ratio</t>
+  </si>
+  <si>
+    <t>BernadoLedoit_Ratio_test</t>
+  </si>
+  <si>
+    <t>Test BernadoLedoit_Ratio</t>
+  </si>
+  <si>
+    <t>Bernado and Ledoit Ratio</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1274,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1273,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2430,6 +2439,17 @@
         <v>307</v>
       </c>
     </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>312</v>
+      </c>
+      <c r="B105" t="s">
+        <v>311</v>
+      </c>
+      <c r="C105" t="s">
+        <v>310</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Add tests to upside_risk macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="322">
   <si>
     <t>Test</t>
   </si>
@@ -958,6 +958,33 @@
   </si>
   <si>
     <t>Bernado and Ledoit Ratio</t>
+  </si>
+  <si>
+    <t>upside_risk_test1</t>
+  </si>
+  <si>
+    <t>Test upside potential for full observations</t>
+  </si>
+  <si>
+    <t>upside risk1</t>
+  </si>
+  <si>
+    <t>upside risk2</t>
+  </si>
+  <si>
+    <t>upside risk3</t>
+  </si>
+  <si>
+    <t>Test upside risk for subset observations</t>
+  </si>
+  <si>
+    <t>Test upside variance for full observations</t>
+  </si>
+  <si>
+    <t>upside_risk_test2</t>
+  </si>
+  <si>
+    <t>upside_risk_test3</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1301,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1282,16 +1309,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2448,6 +2475,39 @@
       </c>
       <c r="C105" t="s">
         <v>310</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>315</v>
+      </c>
+      <c r="B106" t="s">
+        <v>314</v>
+      </c>
+      <c r="C106" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>316</v>
+      </c>
+      <c r="B107" t="s">
+        <v>318</v>
+      </c>
+      <c r="C107" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>317</v>
+      </c>
+      <c r="B108" t="s">
+        <v>319</v>
+      </c>
+      <c r="C108" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test added for Kappa, KellyRatio, SortinoRatio
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rma\Desktop\mytest\SASPerformanceAnalytics\Performance Analytics Library\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19716" windowHeight="8004"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="331">
   <si>
     <t>Test</t>
   </si>
@@ -958,6 +963,60 @@
   </si>
   <si>
     <t>Bernado and Ledoit Ratio</t>
+  </si>
+  <si>
+    <t>Kappa1</t>
+  </si>
+  <si>
+    <t>Test Kappa with L=1</t>
+  </si>
+  <si>
+    <t>Kappa_test1</t>
+  </si>
+  <si>
+    <t>Kappa2</t>
+  </si>
+  <si>
+    <t>Test Kappa with L=2</t>
+  </si>
+  <si>
+    <t>Kappa_test2</t>
+  </si>
+  <si>
+    <t>SortinoRatio1</t>
+  </si>
+  <si>
+    <t>Test SortinoRatio with group=FULL</t>
+  </si>
+  <si>
+    <t>SortinoRatio_test1</t>
+  </si>
+  <si>
+    <t>SortinoRatio2</t>
+  </si>
+  <si>
+    <t>Test SortinoRatio with group=SUBSET</t>
+  </si>
+  <si>
+    <t>SortinoRatio_test2</t>
+  </si>
+  <si>
+    <t>KellyRatio1</t>
+  </si>
+  <si>
+    <t>Test KellyRatio with method=half</t>
+  </si>
+  <si>
+    <t>KellyRatio_test1</t>
+  </si>
+  <si>
+    <t>KellyRatio2</t>
+  </si>
+  <si>
+    <t>Test KellyRatio with method=full</t>
+  </si>
+  <si>
+    <t>KellyRatio_test2</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1333,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1282,20 +1341,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1306,7 +1365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -1317,7 +1376,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1328,7 +1387,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1339,7 +1398,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -1350,7 +1409,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>211</v>
       </c>
@@ -1361,7 +1420,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>265</v>
       </c>
@@ -1372,7 +1431,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>268</v>
       </c>
@@ -1383,7 +1442,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>161</v>
       </c>
@@ -1394,7 +1453,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>162</v>
       </c>
@@ -1405,7 +1464,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>163</v>
       </c>
@@ -1416,7 +1475,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>257</v>
       </c>
@@ -1427,7 +1486,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>131</v>
       </c>
@@ -1438,7 +1497,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -1449,7 +1508,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>135</v>
       </c>
@@ -1460,7 +1519,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -1471,7 +1530,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>223</v>
       </c>
@@ -1482,7 +1541,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>225</v>
       </c>
@@ -1493,7 +1552,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1504,7 +1563,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>166</v>
       </c>
@@ -1515,7 +1574,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>125</v>
       </c>
@@ -1526,7 +1585,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -1537,7 +1596,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>260</v>
       </c>
@@ -1548,7 +1607,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>252</v>
       </c>
@@ -1559,7 +1618,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>261</v>
       </c>
@@ -1570,7 +1629,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>242</v>
       </c>
@@ -1581,7 +1640,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>243</v>
       </c>
@@ -1592,7 +1651,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>156</v>
       </c>
@@ -1603,7 +1662,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -1614,7 +1673,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -1625,7 +1684,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>217</v>
       </c>
@@ -1636,7 +1695,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>219</v>
       </c>
@@ -1647,7 +1706,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>203</v>
       </c>
@@ -1658,7 +1717,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -1669,7 +1728,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -1680,7 +1739,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>172</v>
       </c>
@@ -1691,7 +1750,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>173</v>
       </c>
@@ -1702,7 +1761,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>236</v>
       </c>
@@ -1713,7 +1772,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1724,7 +1783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1735,7 +1794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -1746,7 +1805,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1757,7 +1816,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -1768,7 +1827,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -1779,7 +1838,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>158</v>
       </c>
@@ -1790,7 +1849,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -1801,7 +1860,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -1812,7 +1871,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>109</v>
       </c>
@@ -1823,7 +1882,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>110</v>
       </c>
@@ -1834,7 +1893,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -1845,7 +1904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -1856,7 +1915,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -1867,7 +1926,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -1878,7 +1937,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -1889,7 +1948,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -1900,7 +1959,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -1911,7 +1970,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -1922,7 +1981,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -1933,7 +1992,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -1944,7 +2003,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -1955,7 +2014,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>246</v>
       </c>
@@ -1966,7 +2025,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -1977,7 +2036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -1988,7 +2047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>212</v>
       </c>
@@ -1999,7 +2058,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>213</v>
       </c>
@@ -2010,7 +2069,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>228</v>
       </c>
@@ -2021,7 +2080,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>231</v>
       </c>
@@ -2032,7 +2091,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -2043,7 +2102,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>139</v>
       </c>
@@ -2054,7 +2113,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>174</v>
       </c>
@@ -2065,7 +2124,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>175</v>
       </c>
@@ -2076,7 +2135,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>176</v>
       </c>
@@ -2087,7 +2146,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>177</v>
       </c>
@@ -2098,7 +2157,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>185</v>
       </c>
@@ -2109,7 +2168,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>196</v>
       </c>
@@ -2120,7 +2179,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>199</v>
       </c>
@@ -2131,7 +2190,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -2142,7 +2201,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>187</v>
       </c>
@@ -2153,7 +2212,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>194</v>
       </c>
@@ -2164,7 +2223,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>118</v>
       </c>
@@ -2175,7 +2234,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2186,7 +2245,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>251</v>
       </c>
@@ -2197,7 +2256,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>37</v>
       </c>
@@ -2208,7 +2267,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -2219,7 +2278,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>33</v>
       </c>
@@ -2230,7 +2289,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>205</v>
       </c>
@@ -2241,7 +2300,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>207</v>
       </c>
@@ -2252,7 +2311,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>143</v>
       </c>
@@ -2263,7 +2322,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>146</v>
       </c>
@@ -2274,7 +2333,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>68</v>
       </c>
@@ -2285,7 +2344,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>121</v>
       </c>
@@ -2296,7 +2355,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>237</v>
       </c>
@@ -2307,7 +2366,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>279</v>
       </c>
@@ -2318,7 +2377,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>281</v>
       </c>
@@ -2329,7 +2388,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>282</v>
       </c>
@@ -2340,7 +2399,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>210</v>
       </c>
@@ -2351,7 +2410,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>214</v>
       </c>
@@ -2362,7 +2421,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>291</v>
       </c>
@@ -2373,7 +2432,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>292</v>
       </c>
@@ -2384,7 +2443,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>295</v>
       </c>
@@ -2395,7 +2454,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>298</v>
       </c>
@@ -2406,7 +2465,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>302</v>
       </c>
@@ -2417,7 +2476,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>304</v>
       </c>
@@ -2428,7 +2487,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>309</v>
       </c>
@@ -2439,7 +2498,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>312</v>
       </c>
@@ -2448,6 +2507,72 @@
       </c>
       <c r="C105" t="s">
         <v>310</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>313</v>
+      </c>
+      <c r="B106" t="s">
+        <v>314</v>
+      </c>
+      <c r="C106" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>316</v>
+      </c>
+      <c r="B107" t="s">
+        <v>317</v>
+      </c>
+      <c r="C107" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>319</v>
+      </c>
+      <c r="B108" t="s">
+        <v>320</v>
+      </c>
+      <c r="C108" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>322</v>
+      </c>
+      <c r="B109" t="s">
+        <v>323</v>
+      </c>
+      <c r="C109" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>325</v>
+      </c>
+      <c r="B110" t="s">
+        <v>326</v>
+      </c>
+      <c r="C110" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>328</v>
+      </c>
+      <c r="B111" t="s">
+        <v>329</v>
+      </c>
+      <c r="C111" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created UpDownRatios and added test
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="334">
   <si>
     <t>Test</t>
   </si>
@@ -1017,6 +1017,15 @@
   </si>
   <si>
     <t>KellyRatio_test2</t>
+  </si>
+  <si>
+    <t>UpDownRatios</t>
+  </si>
+  <si>
+    <t>Test UpDownRatios</t>
+  </si>
+  <si>
+    <t>UpDownRatios_test</t>
   </si>
 </sst>
 </file>
@@ -1341,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100"/>
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2575,6 +2584,17 @@
         <v>330</v>
       </c>
     </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>331</v>
+      </c>
+      <c r="B112" t="s">
+        <v>332</v>
+      </c>
+      <c r="C112" t="s">
+        <v>333</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Add tests to downside_risk macro
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="331">
   <si>
     <t>Test</t>
   </si>
@@ -963,9 +963,6 @@
     <t>upside_risk_test1</t>
   </si>
   <si>
-    <t>Test upside potential for full observations</t>
-  </si>
-  <si>
     <t>upside risk1</t>
   </si>
   <si>
@@ -985,6 +982,36 @@
   </si>
   <si>
     <t>upside_risk_test3</t>
+  </si>
+  <si>
+    <t>Test upside potential for subset observations</t>
+  </si>
+  <si>
+    <t>downside risk1</t>
+  </si>
+  <si>
+    <t>Test downside potential for full observations</t>
+  </si>
+  <si>
+    <t>downside_risk_test1</t>
+  </si>
+  <si>
+    <t>downside risk2</t>
+  </si>
+  <si>
+    <t>downside risk3</t>
+  </si>
+  <si>
+    <t>Test downside risk for full observations</t>
+  </si>
+  <si>
+    <t>downside_risk_test2</t>
+  </si>
+  <si>
+    <t>Test downside risk for subset observations</t>
+  </si>
+  <si>
+    <t>downside_risk_test3</t>
   </si>
 </sst>
 </file>
@@ -1309,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2479,10 +2506,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B106" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="C106" t="s">
         <v>313</v>
@@ -2490,24 +2517,57 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B107" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C107" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B108" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C108" t="s">
-        <v>321</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>322</v>
+      </c>
+      <c r="B109" t="s">
+        <v>323</v>
+      </c>
+      <c r="C109" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>325</v>
+      </c>
+      <c r="B110" t="s">
+        <v>327</v>
+      </c>
+      <c r="C110" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>326</v>
+      </c>
+      <c r="B111" t="s">
+        <v>329</v>
+      </c>
+      <c r="C111" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created downside_frequency and upside_frequency macros and added tests
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="358">
   <si>
     <t>Test</t>
   </si>
@@ -1075,6 +1075,24 @@
   </si>
   <si>
     <t>Kappa1</t>
+  </si>
+  <si>
+    <t>downside frequency</t>
+  </si>
+  <si>
+    <t>Test downside frequency</t>
+  </si>
+  <si>
+    <t>downside_frequency_test</t>
+  </si>
+  <si>
+    <t>upside frequency</t>
+  </si>
+  <si>
+    <t>Test upside frequency</t>
+  </si>
+  <si>
+    <t>upside_frequency_test</t>
   </si>
 </sst>
 </file>
@@ -1399,10 +1417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C118"/>
+  <dimension ref="A1:C120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122"/>
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2710,6 +2728,28 @@
         <v>330</v>
       </c>
     </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>352</v>
+      </c>
+      <c r="B119" t="s">
+        <v>353</v>
+      </c>
+      <c r="C119" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>355</v>
+      </c>
+      <c r="B120" t="s">
+        <v>356</v>
+      </c>
+      <c r="C120" t="s">
+        <v>357</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Table_CaptureRatios and Table_UpDownRatios created and tested
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="340">
   <si>
     <t>Test</t>
   </si>
@@ -1026,6 +1026,24 @@
   </si>
   <si>
     <t>UpDownRatios_test</t>
+  </si>
+  <si>
+    <t>Table_CaptureRatios</t>
+  </si>
+  <si>
+    <t>Test Table_CaptureRatios</t>
+  </si>
+  <si>
+    <t>Table_CaptureRatios_test</t>
+  </si>
+  <si>
+    <t>Table_UpDownRatios</t>
+  </si>
+  <si>
+    <t>Test Table_UpDownRatios</t>
+  </si>
+  <si>
+    <t>Table_UpDownTatios_test</t>
   </si>
 </sst>
 </file>
@@ -1350,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+      <selection activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2595,6 +2613,28 @@
         <v>333</v>
       </c>
     </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>334</v>
+      </c>
+      <c r="B113" t="s">
+        <v>335</v>
+      </c>
+      <c r="C113" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>337</v>
+      </c>
+      <c r="B114" t="s">
+        <v>338</v>
+      </c>
+      <c r="C114" t="s">
+        <v>339</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Revert "Table_CaptureRatios and Table_UpDownRatios created and tested"
This reverts commit 95a49eaa650cc182855fe25cc024c6d8244c7090.
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="334">
   <si>
     <t>Test</t>
   </si>
@@ -1026,24 +1026,6 @@
   </si>
   <si>
     <t>UpDownRatios_test</t>
-  </si>
-  <si>
-    <t>Table_CaptureRatios</t>
-  </si>
-  <si>
-    <t>Test Table_CaptureRatios</t>
-  </si>
-  <si>
-    <t>Table_CaptureRatios_test</t>
-  </si>
-  <si>
-    <t>Table_UpDownRatios</t>
-  </si>
-  <si>
-    <t>Test Table_UpDownRatios</t>
-  </si>
-  <si>
-    <t>Table_UpDownTatios_test</t>
   </si>
 </sst>
 </file>
@@ -1368,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2613,28 +2595,6 @@
         <v>333</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>334</v>
-      </c>
-      <c r="B113" t="s">
-        <v>335</v>
-      </c>
-      <c r="C113" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>337</v>
-      </c>
-      <c r="B114" t="s">
-        <v>338</v>
-      </c>
-      <c r="C114" t="s">
-        <v>339</v>
-      </c>
-    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
Created UpsidePotentialRatio macro and added tests
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="364">
   <si>
     <t>Test</t>
   </si>
@@ -1093,6 +1093,24 @@
   </si>
   <si>
     <t>upside_frequency_test</t>
+  </si>
+  <si>
+    <t>UpsidePotentialRatio_test2</t>
+  </si>
+  <si>
+    <t>Test upside potential ratio for full sets</t>
+  </si>
+  <si>
+    <t>UpsidePotentialRatio2</t>
+  </si>
+  <si>
+    <t>UpsidePotentialRatio1</t>
+  </si>
+  <si>
+    <t>Test upside potential ratio for subsets</t>
+  </si>
+  <si>
+    <t>UpsidePotentialRatio_test1</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1427,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1417,10 +1435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2750,6 +2768,28 @@
         <v>357</v>
       </c>
     </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>361</v>
+      </c>
+      <c r="B121" t="s">
+        <v>362</v>
+      </c>
+      <c r="C121" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>360</v>
+      </c>
+      <c r="B122" t="s">
+        <v>359</v>
+      </c>
+      <c r="C122" t="s">
+        <v>358</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
add prospect ratio test in tests.xlsx
</commit_message>
<xml_diff>
--- a/Performance Analytics Library/test/tests.xlsx
+++ b/Performance Analytics Library/test/tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="379">
   <si>
     <t>Test</t>
   </si>
@@ -1152,6 +1152,15 @@
   </si>
   <si>
     <t>Test BernardoLedoit_Ratio</t>
+  </si>
+  <si>
+    <t>Prospect_Ratio_test</t>
+  </si>
+  <si>
+    <t>Prospect_Ratio</t>
+  </si>
+  <si>
+    <t>Test Prospect Ratio</t>
   </si>
 </sst>
 </file>
@@ -1476,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C126"/>
+  <dimension ref="A1:C127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,6 +2884,17 @@
         <v>372</v>
       </c>
     </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>377</v>
+      </c>
+      <c r="B127" t="s">
+        <v>378</v>
+      </c>
+      <c r="C127" t="s">
+        <v>376</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C95">
     <sortCondition ref="A1"/>

</xml_diff>